<commit_message>
Actualización automática 2025-05-30 08:25:07
</commit_message>
<xml_diff>
--- a/data/STROBEL CORDERO MARIA ELISABETH.xlsx
+++ b/data/STROBEL CORDERO MARIA ELISABETH.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N262"/>
+  <dimension ref="A1:N263"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12006,12 +12006,12 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
+          <t>PAREDES AGUILAR ILIANA GABRIELA</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>BARRAGAN PUENTE NATALY CAROLINA</t>
+          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
         </is>
       </c>
       <c r="C241" s="2" t="n">
@@ -12059,7 +12059,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>BECERRA FARIAS ROSA DAYANA</t>
+          <t>BARRAGAN PUENTE NATALY CAROLINA</t>
         </is>
       </c>
       <c r="C242" s="2" t="n">
@@ -12107,7 +12107,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>BELTRAN ESPINOZA SONIA SARITA</t>
+          <t>BECERRA FARIAS ROSA DAYANA</t>
         </is>
       </c>
       <c r="C243" s="2" t="n">
@@ -12155,7 +12155,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>CAIZA COLLAGUAZO ROCIO PILAR</t>
+          <t>BELTRAN ESPINOZA SONIA SARITA</t>
         </is>
       </c>
       <c r="C244" s="2" t="n">
@@ -12203,7 +12203,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>CERAMICAS AL COSTO S.A.S.</t>
+          <t>CAIZA COLLAGUAZO ROCIO PILAR</t>
         </is>
       </c>
       <c r="C245" s="2" t="n">
@@ -12234,7 +12234,7 @@
         <v>0</v>
       </c>
       <c r="L245" s="2" t="n">
-        <v>11287.86</v>
+        <v>0</v>
       </c>
       <c r="M245" s="2" t="n">
         <v>0</v>
@@ -12251,7 +12251,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>CERAMICCENTER CIA. LTDA.</t>
+          <t>CERAMICAS AL COSTO S.A.S.</t>
         </is>
       </c>
       <c r="C246" s="2" t="n">
@@ -12282,7 +12282,7 @@
         <v>0</v>
       </c>
       <c r="L246" s="2" t="n">
-        <v>0</v>
+        <v>11287.86</v>
       </c>
       <c r="M246" s="2" t="n">
         <v>0</v>
@@ -12299,7 +12299,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>CONZA VEGA FRANCO BLADYMIR</t>
+          <t>CERAMICCENTER CIA. LTDA.</t>
         </is>
       </c>
       <c r="C247" s="2" t="n">
@@ -12330,7 +12330,7 @@
         <v>0</v>
       </c>
       <c r="L247" s="2" t="n">
-        <v>1183.91</v>
+        <v>0</v>
       </c>
       <c r="M247" s="2" t="n">
         <v>0</v>
@@ -12347,7 +12347,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>DDH S.A.S.</t>
+          <t>CONZA VEGA FRANCO BLADYMIR</t>
         </is>
       </c>
       <c r="C248" s="2" t="n">
@@ -12378,7 +12378,7 @@
         <v>0</v>
       </c>
       <c r="L248" s="2" t="n">
-        <v>0</v>
+        <v>1183.91</v>
       </c>
       <c r="M248" s="2" t="n">
         <v>0</v>
@@ -12395,7 +12395,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>F.V - AREA ANDINA S.A.</t>
+          <t>DDH S.A.S.</t>
         </is>
       </c>
       <c r="C249" s="2" t="n">
@@ -12426,7 +12426,7 @@
         <v>0</v>
       </c>
       <c r="L249" s="2" t="n">
-        <v>5556.96</v>
+        <v>0</v>
       </c>
       <c r="M249" s="2" t="n">
         <v>0</v>
@@ -12443,7 +12443,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>FERRIACABADOS MACONSE</t>
+          <t>F.V - AREA ANDINA S.A.</t>
         </is>
       </c>
       <c r="C250" s="2" t="n">
@@ -12474,7 +12474,7 @@
         <v>0</v>
       </c>
       <c r="L250" s="2" t="n">
-        <v>0</v>
+        <v>5556.96</v>
       </c>
       <c r="M250" s="2" t="n">
         <v>0</v>
@@ -12491,7 +12491,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>GANCHOZO CEDEÑO YURI MERCEDES</t>
+          <t>FERRIACABADOS MACONSE</t>
         </is>
       </c>
       <c r="C251" s="2" t="n">
@@ -12539,7 +12539,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>MUNDO-CERAMICO CIA.LTDA.</t>
+          <t>GANCHOZO CEDEÑO YURI MERCEDES</t>
         </is>
       </c>
       <c r="C252" s="2" t="n">
@@ -12587,7 +12587,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>TAMAYO VILLACIS EDWIN XAVIER</t>
+          <t>MUNDO-CERAMICO CIA.LTDA.</t>
         </is>
       </c>
       <c r="C253" s="2" t="n">
@@ -12635,7 +12635,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>TOSCANO RAMIREZ MONICA CECILIA</t>
+          <t>TAMAYO VILLACIS EDWIN XAVIER</t>
         </is>
       </c>
       <c r="C254" s="2" t="n">
@@ -12683,7 +12683,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>VELASQUEZ ARELLANO SAIRA MAGDALENA</t>
+          <t>TOSCANO RAMIREZ MONICA CECILIA</t>
         </is>
       </c>
       <c r="C255" s="2" t="n">
@@ -12731,7 +12731,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>VIDAL VARGAS ANDREA DOMINIQUE</t>
+          <t>VELASQUEZ ARELLANO SAIRA MAGDALENA</t>
         </is>
       </c>
       <c r="C256" s="2" t="n">
@@ -12779,14 +12779,14 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>ZAMBRANO ANGELA MARIA</t>
+          <t>VIDAL VARGAS ANDREA DOMINIQUE</t>
         </is>
       </c>
       <c r="C257" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D257" s="2" t="n">
-        <v>7441.92</v>
+        <v>0</v>
       </c>
       <c r="E257" s="2" t="n">
         <v>0</v>
@@ -12822,19 +12822,19 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>VACA PANCHI CAROLINA</t>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>AGUILERA ANDRADE FAUSTO ROGELIO</t>
+          <t>ZAMBRANO ANGELA MARIA</t>
         </is>
       </c>
       <c r="C258" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D258" s="2" t="n">
-        <v>0</v>
+        <v>7441.92</v>
       </c>
       <c r="E258" s="2" t="n">
         <v>0</v>
@@ -12875,7 +12875,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>ARCOS GOMEZ CONSTRUCCIONES CIA. LTDA.</t>
+          <t>AGUILERA ANDRADE FAUSTO ROGELIO</t>
         </is>
       </c>
       <c r="C259" s="2" t="n">
@@ -12923,7 +12923,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>CARRION ALVAREZ MARIO ANDRES</t>
+          <t>ARCOS GOMEZ CONSTRUCCIONES CIA. LTDA.</t>
         </is>
       </c>
       <c r="C260" s="2" t="n">
@@ -12971,105 +12971,153 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
+          <t>CARRION ALVAREZ MARIO ANDRES</t>
+        </is>
+      </c>
+      <c r="C261" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D261" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E261" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F261" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G261" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H261" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I261" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J261" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K261" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L261" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M261" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N261" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>VACA PANCHI CAROLINA</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
           <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
-      <c r="C261" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D261" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E261" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F261" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G261" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H261" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I261" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J261" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K261" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L261" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M261" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N261" s="2" t="n">
+      <c r="C262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N262" s="2" t="n">
         <v>3.46</v>
       </c>
     </row>
-    <row r="262">
-      <c r="C262" s="3" t="inlineStr">
-        <is>
-          <t>2 de 260</t>
-        </is>
-      </c>
-      <c r="D262" s="3" t="inlineStr">
-        <is>
-          <t>24 de 260</t>
-        </is>
-      </c>
-      <c r="E262" s="3" t="inlineStr">
-        <is>
-          <t>5 de 260</t>
-        </is>
-      </c>
-      <c r="F262" s="3" t="inlineStr">
-        <is>
-          <t>1 de 260</t>
-        </is>
-      </c>
-      <c r="G262" s="3" t="inlineStr">
-        <is>
-          <t>4 de 260</t>
-        </is>
-      </c>
-      <c r="H262" s="3" t="inlineStr">
-        <is>
-          <t>3 de 260</t>
-        </is>
-      </c>
-      <c r="I262" s="3" t="inlineStr">
-        <is>
-          <t>2 de 260</t>
-        </is>
-      </c>
-      <c r="J262" s="3" t="inlineStr">
-        <is>
-          <t>5 de 260</t>
-        </is>
-      </c>
-      <c r="K262" s="3" t="inlineStr">
-        <is>
-          <t>21 de 260</t>
-        </is>
-      </c>
-      <c r="L262" s="3" t="inlineStr">
-        <is>
-          <t>57 de 260</t>
-        </is>
-      </c>
-      <c r="M262" s="3" t="inlineStr">
-        <is>
-          <t>3 de 260</t>
-        </is>
-      </c>
-      <c r="N262" s="3" t="inlineStr">
-        <is>
-          <t>5 de 260</t>
+    <row r="263">
+      <c r="C263" s="3" t="inlineStr">
+        <is>
+          <t>2 de 261</t>
+        </is>
+      </c>
+      <c r="D263" s="3" t="inlineStr">
+        <is>
+          <t>24 de 261</t>
+        </is>
+      </c>
+      <c r="E263" s="3" t="inlineStr">
+        <is>
+          <t>5 de 261</t>
+        </is>
+      </c>
+      <c r="F263" s="3" t="inlineStr">
+        <is>
+          <t>1 de 261</t>
+        </is>
+      </c>
+      <c r="G263" s="3" t="inlineStr">
+        <is>
+          <t>4 de 261</t>
+        </is>
+      </c>
+      <c r="H263" s="3" t="inlineStr">
+        <is>
+          <t>3 de 261</t>
+        </is>
+      </c>
+      <c r="I263" s="3" t="inlineStr">
+        <is>
+          <t>2 de 261</t>
+        </is>
+      </c>
+      <c r="J263" s="3" t="inlineStr">
+        <is>
+          <t>5 de 261</t>
+        </is>
+      </c>
+      <c r="K263" s="3" t="inlineStr">
+        <is>
+          <t>21 de 261</t>
+        </is>
+      </c>
+      <c r="L263" s="3" t="inlineStr">
+        <is>
+          <t>57 de 261</t>
+        </is>
+      </c>
+      <c r="M263" s="3" t="inlineStr">
+        <is>
+          <t>3 de 261</t>
+        </is>
+      </c>
+      <c r="N263" s="3" t="inlineStr">
+        <is>
+          <t>5 de 261</t>
         </is>
       </c>
     </row>
@@ -13084,7 +13132,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F262"/>
+  <dimension ref="A1:F263"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18871,12 +18919,12 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
+          <t>PAREDES AGUILAR ILIANA GABRIELA</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>BARRAGAN PUENTE NATALY CAROLINA</t>
+          <t>CONSTRUCCION, INGENIERIA Y TECNOLOGIA CONSTRUINTEC SAS</t>
         </is>
       </c>
       <c r="C241" s="2" t="n">
@@ -18889,7 +18937,7 @@
         <v>0</v>
       </c>
       <c r="F241" s="2" t="n">
-        <v>-49.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242">
@@ -18900,7 +18948,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>BECERRA FARIAS ROSA DAYANA</t>
+          <t>BARRAGAN PUENTE NATALY CAROLINA</t>
         </is>
       </c>
       <c r="C242" s="2" t="n">
@@ -18913,7 +18961,7 @@
         <v>0</v>
       </c>
       <c r="F242" s="2" t="n">
-        <v>3054.27</v>
+        <v>-49.25</v>
       </c>
     </row>
     <row r="243">
@@ -18924,7 +18972,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>BELTRAN ESPINOZA SONIA SARITA</t>
+          <t>BECERRA FARIAS ROSA DAYANA</t>
         </is>
       </c>
       <c r="C243" s="2" t="n">
@@ -18937,7 +18985,7 @@
         <v>0</v>
       </c>
       <c r="F243" s="2" t="n">
-        <v>0</v>
+        <v>3054.27</v>
       </c>
     </row>
     <row r="244">
@@ -18948,11 +18996,11 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>CAIZA COLLAGUAZO ROCIO PILAR</t>
+          <t>BELTRAN ESPINOZA SONIA SARITA</t>
         </is>
       </c>
       <c r="C244" s="2" t="n">
-        <v>3687.82</v>
+        <v>0</v>
       </c>
       <c r="D244" s="2" t="n">
         <v>0</v>
@@ -18961,7 +19009,7 @@
         <v>0</v>
       </c>
       <c r="F244" s="2" t="n">
-        <v>226.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="245">
@@ -18972,20 +19020,20 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>CERAMICAS AL COSTO S.A.S.</t>
+          <t>CAIZA COLLAGUAZO ROCIO PILAR</t>
         </is>
       </c>
       <c r="C245" s="2" t="n">
-        <v>-289.82</v>
+        <v>3687.82</v>
       </c>
       <c r="D245" s="2" t="n">
-        <v>1728.53</v>
+        <v>0</v>
       </c>
       <c r="E245" s="2" t="n">
-        <v>11287.86</v>
+        <v>0</v>
       </c>
       <c r="F245" s="2" t="n">
-        <v>2867.6</v>
+        <v>226.8</v>
       </c>
     </row>
     <row r="246">
@@ -18996,20 +19044,20 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>CERAMICCENTER CIA. LTDA.</t>
+          <t>CERAMICAS AL COSTO S.A.S.</t>
         </is>
       </c>
       <c r="C246" s="2" t="n">
-        <v>0</v>
+        <v>-289.82</v>
       </c>
       <c r="D246" s="2" t="n">
-        <v>0</v>
+        <v>1728.53</v>
       </c>
       <c r="E246" s="2" t="n">
-        <v>0</v>
+        <v>11287.86</v>
       </c>
       <c r="F246" s="2" t="n">
-        <v>0</v>
+        <v>2867.6</v>
       </c>
     </row>
     <row r="247">
@@ -19020,20 +19068,20 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>CONZA VEGA FRANCO BLADYMIR</t>
+          <t>CERAMICCENTER CIA. LTDA.</t>
         </is>
       </c>
       <c r="C247" s="2" t="n">
-        <v>939.59</v>
+        <v>0</v>
       </c>
       <c r="D247" s="2" t="n">
-        <v>-266.91</v>
+        <v>0</v>
       </c>
       <c r="E247" s="2" t="n">
-        <v>1183.91</v>
+        <v>0</v>
       </c>
       <c r="F247" s="2" t="n">
-        <v>2785.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="248">
@@ -19044,20 +19092,20 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>DDH S.A.S.</t>
+          <t>CONZA VEGA FRANCO BLADYMIR</t>
         </is>
       </c>
       <c r="C248" s="2" t="n">
-        <v>-244.14</v>
+        <v>939.59</v>
       </c>
       <c r="D248" s="2" t="n">
-        <v>4896.51</v>
+        <v>-266.91</v>
       </c>
       <c r="E248" s="2" t="n">
-        <v>0</v>
+        <v>1183.91</v>
       </c>
       <c r="F248" s="2" t="n">
-        <v>0</v>
+        <v>2785.1</v>
       </c>
     </row>
     <row r="249">
@@ -19068,20 +19116,20 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>F.V - AREA ANDINA S.A.</t>
+          <t>DDH S.A.S.</t>
         </is>
       </c>
       <c r="C249" s="2" t="n">
-        <v>4883.76</v>
+        <v>-244.14</v>
       </c>
       <c r="D249" s="2" t="n">
-        <v>8752.889999999999</v>
+        <v>4896.51</v>
       </c>
       <c r="E249" s="2" t="n">
-        <v>5556.96</v>
+        <v>0</v>
       </c>
       <c r="F249" s="2" t="n">
-        <v>156.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="250">
@@ -19092,20 +19140,20 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>FERRIACABADOS MACONSE</t>
+          <t>F.V - AREA ANDINA S.A.</t>
         </is>
       </c>
       <c r="C250" s="2" t="n">
-        <v>0</v>
+        <v>4883.76</v>
       </c>
       <c r="D250" s="2" t="n">
-        <v>0</v>
+        <v>8752.889999999999</v>
       </c>
       <c r="E250" s="2" t="n">
-        <v>0</v>
+        <v>5556.96</v>
       </c>
       <c r="F250" s="2" t="n">
-        <v>0</v>
+        <v>156.67</v>
       </c>
     </row>
     <row r="251">
@@ -19116,14 +19164,14 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>GANCHOZO CEDEÑO YURI MERCEDES</t>
+          <t>FERRIACABADOS MACONSE</t>
         </is>
       </c>
       <c r="C251" s="2" t="n">
-        <v>1297.61</v>
+        <v>0</v>
       </c>
       <c r="D251" s="2" t="n">
-        <v>648.8099999999999</v>
+        <v>0</v>
       </c>
       <c r="E251" s="2" t="n">
         <v>0</v>
@@ -19140,14 +19188,14 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>MUNDO-CERAMICO CIA.LTDA.</t>
+          <t>GANCHOZO CEDEÑO YURI MERCEDES</t>
         </is>
       </c>
       <c r="C252" s="2" t="n">
-        <v>0</v>
+        <v>1297.61</v>
       </c>
       <c r="D252" s="2" t="n">
-        <v>0</v>
+        <v>648.8099999999999</v>
       </c>
       <c r="E252" s="2" t="n">
         <v>0</v>
@@ -19164,7 +19212,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>TAMAYO VILLACIS EDWIN XAVIER</t>
+          <t>MUNDO-CERAMICO CIA.LTDA.</t>
         </is>
       </c>
       <c r="C253" s="2" t="n">
@@ -19177,7 +19225,7 @@
         <v>0</v>
       </c>
       <c r="F253" s="2" t="n">
-        <v>40.19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="254">
@@ -19188,11 +19236,11 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>TOSCANO RAMIREZ MONICA CECILIA</t>
+          <t>TAMAYO VILLACIS EDWIN XAVIER</t>
         </is>
       </c>
       <c r="C254" s="2" t="n">
-        <v>3216.09</v>
+        <v>0</v>
       </c>
       <c r="D254" s="2" t="n">
         <v>0</v>
@@ -19201,7 +19249,7 @@
         <v>0</v>
       </c>
       <c r="F254" s="2" t="n">
-        <v>0</v>
+        <v>40.19</v>
       </c>
     </row>
     <row r="255">
@@ -19212,11 +19260,11 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>VELASQUEZ ARELLANO SAIRA MAGDALENA</t>
+          <t>TOSCANO RAMIREZ MONICA CECILIA</t>
         </is>
       </c>
       <c r="C255" s="2" t="n">
-        <v>0</v>
+        <v>3216.09</v>
       </c>
       <c r="D255" s="2" t="n">
         <v>0</v>
@@ -19236,14 +19284,14 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>VIDAL VARGAS ANDREA DOMINIQUE</t>
+          <t>VELASQUEZ ARELLANO SAIRA MAGDALENA</t>
         </is>
       </c>
       <c r="C256" s="2" t="n">
-        <v>320.39</v>
+        <v>0</v>
       </c>
       <c r="D256" s="2" t="n">
-        <v>126.72</v>
+        <v>0</v>
       </c>
       <c r="E256" s="2" t="n">
         <v>0</v>
@@ -19260,44 +19308,44 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>ZAMBRANO ANGELA MARIA</t>
+          <t>VIDAL VARGAS ANDREA DOMINIQUE</t>
         </is>
       </c>
       <c r="C257" s="2" t="n">
-        <v>6051.93</v>
+        <v>320.39</v>
       </c>
       <c r="D257" s="2" t="n">
-        <v>3152.52</v>
+        <v>126.72</v>
       </c>
       <c r="E257" s="2" t="n">
-        <v>7441.92</v>
+        <v>0</v>
       </c>
       <c r="F257" s="2" t="n">
-        <v>8859.700000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>VACA PANCHI CAROLINA</t>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>AGUILERA ANDRADE FAUSTO ROGELIO</t>
+          <t>ZAMBRANO ANGELA MARIA</t>
         </is>
       </c>
       <c r="C258" s="2" t="n">
-        <v>0</v>
+        <v>6051.93</v>
       </c>
       <c r="D258" s="2" t="n">
-        <v>0</v>
+        <v>3152.52</v>
       </c>
       <c r="E258" s="2" t="n">
-        <v>0</v>
+        <v>7441.92</v>
       </c>
       <c r="F258" s="2" t="n">
-        <v>0</v>
+        <v>8859.700000000001</v>
       </c>
     </row>
     <row r="259">
@@ -19308,7 +19356,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>ARCOS GOMEZ CONSTRUCCIONES CIA. LTDA.</t>
+          <t>AGUILERA ANDRADE FAUSTO ROGELIO</t>
         </is>
       </c>
       <c r="C259" s="2" t="n">
@@ -19332,14 +19380,14 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>CARRION ALVAREZ MARIO ANDRES</t>
+          <t>ARCOS GOMEZ CONSTRUCCIONES CIA. LTDA.</t>
         </is>
       </c>
       <c r="C260" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D260" s="2" t="n">
-        <v>12.48</v>
+        <v>0</v>
       </c>
       <c r="E260" s="2" t="n">
         <v>0</v>
@@ -19356,33 +19404,57 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
+          <t>CARRION ALVAREZ MARIO ANDRES</t>
+        </is>
+      </c>
+      <c r="C261" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D261" s="2" t="n">
+        <v>12.48</v>
+      </c>
+      <c r="E261" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F261" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>VACA PANCHI CAROLINA</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
           <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
-      <c r="C261" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D261" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E261" s="2" t="n">
+      <c r="C262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E262" s="2" t="n">
         <v>3.47</v>
       </c>
-      <c r="F261" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="262">
-      <c r="C262" s="4" t="n">
+      <c r="F262" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="C263" s="4" t="n">
         <v>278951.89</v>
       </c>
-      <c r="D262" s="4" t="n">
+      <c r="D263" s="4" t="n">
         <v>353872.81</v>
       </c>
-      <c r="E262" s="4" t="n">
+      <c r="E263" s="4" t="n">
         <v>256699.85</v>
       </c>
-      <c r="F262" s="4" t="n">
+      <c r="F263" s="4" t="n">
         <v>238592.19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-05-30 17:10:07
</commit_message>
<xml_diff>
--- a/data/STROBEL CORDERO MARIA ELISABETH.xlsx
+++ b/data/STROBEL CORDERO MARIA ELISABETH.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N263"/>
+  <dimension ref="A1:N264"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13019,105 +13019,153 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+        </is>
+      </c>
+      <c r="C262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N262" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>VACA PANCHI CAROLINA</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
           <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
-      <c r="C262" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D262" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E262" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F262" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G262" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H262" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I262" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J262" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K262" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L262" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M262" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N262" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="263">
-      <c r="C263" s="3" t="inlineStr">
-        <is>
-          <t>15 de 261</t>
-        </is>
-      </c>
-      <c r="D263" s="3" t="inlineStr">
-        <is>
-          <t>18 de 261</t>
-        </is>
-      </c>
-      <c r="E263" s="3" t="inlineStr">
-        <is>
-          <t>16 de 261</t>
-        </is>
-      </c>
-      <c r="F263" s="3" t="inlineStr">
-        <is>
-          <t>10 de 261</t>
-        </is>
-      </c>
-      <c r="G263" s="3" t="inlineStr">
-        <is>
-          <t>2 de 261</t>
-        </is>
-      </c>
-      <c r="H263" s="3" t="inlineStr">
-        <is>
-          <t>2 de 261</t>
-        </is>
-      </c>
-      <c r="I263" s="3" t="inlineStr">
-        <is>
-          <t>3 de 261</t>
-        </is>
-      </c>
-      <c r="J263" s="3" t="inlineStr">
-        <is>
-          <t>3 de 261</t>
-        </is>
-      </c>
-      <c r="K263" s="3" t="inlineStr">
-        <is>
-          <t>20 de 261</t>
-        </is>
-      </c>
-      <c r="L263" s="3" t="inlineStr">
-        <is>
-          <t>66 de 261</t>
-        </is>
-      </c>
-      <c r="M263" s="3" t="inlineStr">
-        <is>
-          <t>5 de 261</t>
-        </is>
-      </c>
-      <c r="N263" s="3" t="inlineStr">
-        <is>
-          <t>9 de 261</t>
+      <c r="C263" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D263" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E263" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F263" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G263" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H263" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I263" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J263" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K263" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L263" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M263" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N263" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="C264" s="3" t="inlineStr">
+        <is>
+          <t>15 de 262</t>
+        </is>
+      </c>
+      <c r="D264" s="3" t="inlineStr">
+        <is>
+          <t>18 de 262</t>
+        </is>
+      </c>
+      <c r="E264" s="3" t="inlineStr">
+        <is>
+          <t>16 de 262</t>
+        </is>
+      </c>
+      <c r="F264" s="3" t="inlineStr">
+        <is>
+          <t>10 de 262</t>
+        </is>
+      </c>
+      <c r="G264" s="3" t="inlineStr">
+        <is>
+          <t>2 de 262</t>
+        </is>
+      </c>
+      <c r="H264" s="3" t="inlineStr">
+        <is>
+          <t>2 de 262</t>
+        </is>
+      </c>
+      <c r="I264" s="3" t="inlineStr">
+        <is>
+          <t>3 de 262</t>
+        </is>
+      </c>
+      <c r="J264" s="3" t="inlineStr">
+        <is>
+          <t>3 de 262</t>
+        </is>
+      </c>
+      <c r="K264" s="3" t="inlineStr">
+        <is>
+          <t>20 de 262</t>
+        </is>
+      </c>
+      <c r="L264" s="3" t="inlineStr">
+        <is>
+          <t>66 de 262</t>
+        </is>
+      </c>
+      <c r="M264" s="3" t="inlineStr">
+        <is>
+          <t>5 de 262</t>
+        </is>
+      </c>
+      <c r="N264" s="3" t="inlineStr">
+        <is>
+          <t>9 de 262</t>
         </is>
       </c>
     </row>
@@ -13132,7 +13180,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F263"/>
+  <dimension ref="A1:F264"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19428,33 +19476,57 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+        </is>
+      </c>
+      <c r="C262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E262" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F262" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>VACA PANCHI CAROLINA</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
           <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
-      <c r="C262" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D262" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E262" s="2" t="n">
+      <c r="C263" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D263" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E263" s="2" t="n">
         <v>3.47</v>
       </c>
-      <c r="F262" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="263">
-      <c r="C263" s="4" t="n">
+      <c r="F263" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="C264" s="4" t="n">
         <v>278951.89</v>
       </c>
-      <c r="D263" s="4" t="n">
+      <c r="D264" s="4" t="n">
         <v>353872.81</v>
       </c>
-      <c r="E263" s="4" t="n">
+      <c r="E264" s="4" t="n">
         <v>256699.85</v>
       </c>
-      <c r="F263" s="4" t="n">
+      <c r="F264" s="4" t="n">
         <v>318541.04</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-06-05 10:50:06
</commit_message>
<xml_diff>
--- a/data/STROBEL CORDERO MARIA ELISABETH.xlsx
+++ b/data/STROBEL CORDERO MARIA ELISABETH.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="VENTAS POR GRUPO" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="VENTA MENSUAL" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="CUMPLIMIENTO MENSUAL" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -59,7 +58,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -69,10 +68,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -20333,3346 +20328,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F138"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="34" customWidth="1" min="1" max="1"/>
-    <col width="22" customWidth="1" min="2" max="2"/>
-    <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
-    <col width="28" customWidth="1" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ASESOR</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>GRUPO</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>PRESUPUESTO</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>VENTA</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>POR CUMPLIR</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>CUMPLIMIENTO</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>240X120 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>260.285000070615</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>260.285000070615</v>
-      </c>
-      <c r="F2" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>240X80 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>3120.1145</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>3120.1145</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>FREGADEROS DE COCINA</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>646.361575487259</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>646.361575487259</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>GRANITO</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>GRIFERIAS</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="F6" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>INODOROS</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>1260</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>1260</v>
-      </c>
-      <c r="F7" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>LAVABOS</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>625</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>625</v>
-      </c>
-      <c r="F8" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F9" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>NO RESURTIBLES</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="F10" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>PANELES DECORATIVOS</t>
-        </is>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="F12" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>PANELES PU</t>
-        </is>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="F13" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>PANELES PVC</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="F14" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>PIEDRA SINTERIZADA</t>
-        </is>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>527.03</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>527.03</v>
-      </c>
-      <c r="F15" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C16" s="2" t="n">
-        <v>18798.61</v>
-      </c>
-      <c r="D16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>18798.61</v>
-      </c>
-      <c r="F16" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>PUERTAS DE SEGURIDAD</t>
-        </is>
-      </c>
-      <c r="C17" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="F17" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>SAL SOLUBLE</t>
-        </is>
-      </c>
-      <c r="C18" s="2" t="n">
-        <v>1600</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>1600</v>
-      </c>
-      <c r="F18" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>240X120 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C19" s="2" t="n">
-        <v>5820</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>1669.25</v>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>4150.75</v>
-      </c>
-      <c r="F19" s="5" t="n">
-        <v>0.2868127147766323</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>240X80 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C20" s="2" t="n">
-        <v>13728</v>
-      </c>
-      <c r="D20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>13728</v>
-      </c>
-      <c r="F20" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>FREGADEROS DE COCINA</t>
-        </is>
-      </c>
-      <c r="C21" s="2" t="n">
-        <v>646</v>
-      </c>
-      <c r="D21" s="2" t="n">
-        <v>128.74</v>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>517.26</v>
-      </c>
-      <c r="F21" s="5" t="n">
-        <v>0.1992879256965945</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>GRANITO</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="D22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="F22" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>GRIFERIAS</t>
-        </is>
-      </c>
-      <c r="C23" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="D23" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="F23" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>INODOROS</t>
-        </is>
-      </c>
-      <c r="C24" s="2" t="n">
-        <v>2100</v>
-      </c>
-      <c r="D24" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>2100</v>
-      </c>
-      <c r="F24" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>LAVABOS</t>
-        </is>
-      </c>
-      <c r="C25" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D25" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F25" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="C26" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F26" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>NO RESURTIBLES</t>
-        </is>
-      </c>
-      <c r="C27" s="2" t="n">
-        <v>1300.5</v>
-      </c>
-      <c r="D27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>1300.5</v>
-      </c>
-      <c r="F27" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>PANELES DECORATIVOS</t>
-        </is>
-      </c>
-      <c r="C29" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="D29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="F29" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>PANELES PU</t>
-        </is>
-      </c>
-      <c r="C30" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="F30" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>PANELES PVC</t>
-        </is>
-      </c>
-      <c r="C31" s="2" t="n">
-        <v>966</v>
-      </c>
-      <c r="D31" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2" t="n">
-        <v>966</v>
-      </c>
-      <c r="F31" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>PIEDRA SINTERIZADA</t>
-        </is>
-      </c>
-      <c r="C32" s="2" t="n">
-        <v>15690</v>
-      </c>
-      <c r="D32" s="2" t="n">
-        <v>2568.3</v>
-      </c>
-      <c r="E32" s="2" t="n">
-        <v>13121.7</v>
-      </c>
-      <c r="F32" s="5" t="n">
-        <v>0.1636902485659656</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C33" s="2" t="n">
-        <v>45745.689</v>
-      </c>
-      <c r="D33" s="2" t="n">
-        <v>346.47</v>
-      </c>
-      <c r="E33" s="2" t="n">
-        <v>45399.219</v>
-      </c>
-      <c r="F33" s="5" t="n">
-        <v>0.007573828432226697</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>PUERTAS DE SEGURIDAD</t>
-        </is>
-      </c>
-      <c r="C34" s="2" t="n">
-        <v>1142</v>
-      </c>
-      <c r="D34" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" s="2" t="n">
-        <v>1142</v>
-      </c>
-      <c r="F34" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>SAL SOLUBLE</t>
-        </is>
-      </c>
-      <c r="C35" s="2" t="n">
-        <v>1600</v>
-      </c>
-      <c r="D35" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" s="2" t="n">
-        <v>1600</v>
-      </c>
-      <c r="F35" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>240X80 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C36" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D36" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F36" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>FREGADEROS DE COCINA</t>
-        </is>
-      </c>
-      <c r="C37" s="2" t="n">
-        <v>250.631825420901</v>
-      </c>
-      <c r="D37" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" s="2" t="n">
-        <v>250.631825420901</v>
-      </c>
-      <c r="F37" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>GRANITO</t>
-        </is>
-      </c>
-      <c r="C38" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="D38" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="F38" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>GRIFERIAS</t>
-        </is>
-      </c>
-      <c r="C39" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="D39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="F39" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>INODOROS</t>
-        </is>
-      </c>
-      <c r="C40" s="2" t="n">
-        <v>800</v>
-      </c>
-      <c r="D40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" s="2" t="n">
-        <v>800</v>
-      </c>
-      <c r="F40" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>LAVABOS</t>
-        </is>
-      </c>
-      <c r="C41" s="2" t="n">
-        <v>500</v>
-      </c>
-      <c r="D41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" s="2" t="n">
-        <v>500</v>
-      </c>
-      <c r="F41" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="C42" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F42" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>NO RESURTIBLES</t>
-        </is>
-      </c>
-      <c r="C43" s="2" t="n">
-        <v>325.13</v>
-      </c>
-      <c r="D43" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" s="2" t="n">
-        <v>325.13</v>
-      </c>
-      <c r="F43" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" s="2" t="n">
-        <v>851.4299999999999</v>
-      </c>
-      <c r="E44" s="2" t="n">
-        <v>-851.4299999999999</v>
-      </c>
-      <c r="F44" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>PANELES DECORATIVOS</t>
-        </is>
-      </c>
-      <c r="C45" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="D45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="F45" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>PANELES PU</t>
-        </is>
-      </c>
-      <c r="C46" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="D46" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E46" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="F46" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>PANELES PVC</t>
-        </is>
-      </c>
-      <c r="C47" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="D47" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="F47" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C48" s="2" t="n">
-        <v>7774.1</v>
-      </c>
-      <c r="D48" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E48" s="2" t="n">
-        <v>7774.1</v>
-      </c>
-      <c r="F48" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>PUERTAS DE SEGURIDAD</t>
-        </is>
-      </c>
-      <c r="C49" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="D49" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="F49" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>SAL SOLUBLE</t>
-        </is>
-      </c>
-      <c r="C50" s="2" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D50" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E50" s="2" t="n">
-        <v>1500</v>
-      </c>
-      <c r="F50" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>240X120 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C51" s="2" t="n">
-        <v>9970.34304517915</v>
-      </c>
-      <c r="D51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" s="2" t="n">
-        <v>9970.34304517915</v>
-      </c>
-      <c r="F51" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>240X80 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C52" s="2" t="n">
-        <v>27457.0076</v>
-      </c>
-      <c r="D52" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E52" s="2" t="n">
-        <v>27457.0076</v>
-      </c>
-      <c r="F52" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>FREGADEROS DE COCINA</t>
-        </is>
-      </c>
-      <c r="C53" s="2" t="n">
-        <v>1003</v>
-      </c>
-      <c r="D53" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" s="2" t="n">
-        <v>1003</v>
-      </c>
-      <c r="F53" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>GRANITO</t>
-        </is>
-      </c>
-      <c r="C54" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="D54" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="F54" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>GRIFERIAS</t>
-        </is>
-      </c>
-      <c r="C55" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="D55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E55" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="F55" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>INODOROS</t>
-        </is>
-      </c>
-      <c r="C56" s="2" t="n">
-        <v>1400</v>
-      </c>
-      <c r="D56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E56" s="2" t="n">
-        <v>1400</v>
-      </c>
-      <c r="F56" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>LAVABOS</t>
-        </is>
-      </c>
-      <c r="C57" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E57" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F57" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="C58" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E58" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F58" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>NO RESURTIBLES</t>
-        </is>
-      </c>
-      <c r="C59" s="2" t="n">
-        <v>1300.5</v>
-      </c>
-      <c r="D59" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E59" s="2" t="n">
-        <v>1300.5</v>
-      </c>
-      <c r="F59" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C60" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D60" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E60" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F60" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>PANELES DECORATIVOS</t>
-        </is>
-      </c>
-      <c r="C61" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="D61" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E61" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="F61" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>PANELES PU</t>
-        </is>
-      </c>
-      <c r="C62" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="D62" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E62" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="F62" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>PANELES PVC</t>
-        </is>
-      </c>
-      <c r="C63" s="2" t="n">
-        <v>966</v>
-      </c>
-      <c r="D63" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E63" s="2" t="n">
-        <v>966</v>
-      </c>
-      <c r="F63" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>PIEDRA SINTERIZADA</t>
-        </is>
-      </c>
-      <c r="C64" s="2" t="n">
-        <v>13500</v>
-      </c>
-      <c r="D64" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E64" s="2" t="n">
-        <v>13500</v>
-      </c>
-      <c r="F64" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C65" s="2" t="n">
-        <v>32741.45</v>
-      </c>
-      <c r="D65" s="2" t="n">
-        <v>2529.84</v>
-      </c>
-      <c r="E65" s="2" t="n">
-        <v>30211.61</v>
-      </c>
-      <c r="F65" s="5" t="n">
-        <v>0.07726719494707779</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>PUERTAS DE SEGURIDAD</t>
-        </is>
-      </c>
-      <c r="C66" s="2" t="n">
-        <v>684</v>
-      </c>
-      <c r="D66" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E66" s="2" t="n">
-        <v>684</v>
-      </c>
-      <c r="F66" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>SAL SOLUBLE</t>
-        </is>
-      </c>
-      <c r="C67" s="2" t="n">
-        <v>3200</v>
-      </c>
-      <c r="D67" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E67" s="2" t="n">
-        <v>3200</v>
-      </c>
-      <c r="F67" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>240X120 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C68" s="2" t="n">
-        <v>782.465010521559</v>
-      </c>
-      <c r="D68" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E68" s="2" t="n">
-        <v>782.465010521559</v>
-      </c>
-      <c r="F68" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>240X80 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C69" s="2" t="n">
-        <v>4168.07156573679</v>
-      </c>
-      <c r="D69" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E69" s="2" t="n">
-        <v>4168.07156573679</v>
-      </c>
-      <c r="F69" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>FREGADEROS DE COCINA</t>
-        </is>
-      </c>
-      <c r="C70" s="2" t="n">
-        <v>513.831046659336</v>
-      </c>
-      <c r="D70" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E70" s="2" t="n">
-        <v>513.831046659336</v>
-      </c>
-      <c r="F70" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>GRANITO</t>
-        </is>
-      </c>
-      <c r="C71" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="D71" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E71" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="F71" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>GRIFERIAS</t>
-        </is>
-      </c>
-      <c r="C72" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="D72" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E72" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="F72" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>INODOROS</t>
-        </is>
-      </c>
-      <c r="C73" s="2" t="n">
-        <v>1800</v>
-      </c>
-      <c r="D73" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E73" s="2" t="n">
-        <v>1800</v>
-      </c>
-      <c r="F73" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>LAVABOS</t>
-        </is>
-      </c>
-      <c r="C74" s="2" t="n">
-        <v>625</v>
-      </c>
-      <c r="D74" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E74" s="2" t="n">
-        <v>625</v>
-      </c>
-      <c r="F74" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="C75" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D75" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E75" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F75" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>NO RESURTIBLES</t>
-        </is>
-      </c>
-      <c r="C76" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="D76" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E76" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="F76" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C77" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D77" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E77" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F77" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>PANELES DECORATIVOS</t>
-        </is>
-      </c>
-      <c r="C78" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="D78" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E78" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="F78" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>PANELES PU</t>
-        </is>
-      </c>
-      <c r="C79" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="D79" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E79" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="F79" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>PANELES PVC</t>
-        </is>
-      </c>
-      <c r="C80" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="D80" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E80" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="F80" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>PIEDRA SINTERIZADA</t>
-        </is>
-      </c>
-      <c r="C81" s="2" t="n">
-        <v>7465</v>
-      </c>
-      <c r="D81" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E81" s="2" t="n">
-        <v>7465</v>
-      </c>
-      <c r="F81" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C82" s="2" t="n">
-        <v>29532.44</v>
-      </c>
-      <c r="D82" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E82" s="2" t="n">
-        <v>29532.44</v>
-      </c>
-      <c r="F82" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>PUERTAS DE SEGURIDAD</t>
-        </is>
-      </c>
-      <c r="C83" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="D83" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E83" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="F83" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>SAL SOLUBLE</t>
-        </is>
-      </c>
-      <c r="C84" s="2" t="n">
-        <v>2800</v>
-      </c>
-      <c r="D84" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E84" s="2" t="n">
-        <v>2800</v>
-      </c>
-      <c r="F84" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>240X120 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C85" s="2" t="n">
-        <v>672.340305337043</v>
-      </c>
-      <c r="D85" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E85" s="2" t="n">
-        <v>672.340305337043</v>
-      </c>
-      <c r="F85" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>240X80 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C86" s="2" t="n">
-        <v>4992.1832</v>
-      </c>
-      <c r="D86" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E86" s="2" t="n">
-        <v>4992.1832</v>
-      </c>
-      <c r="F86" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>FREGADEROS DE COCINA</t>
-        </is>
-      </c>
-      <c r="C87" s="2" t="n">
-        <v>142.502095025027</v>
-      </c>
-      <c r="D87" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E87" s="2" t="n">
-        <v>142.502095025027</v>
-      </c>
-      <c r="F87" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>GRANITO</t>
-        </is>
-      </c>
-      <c r="C88" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="D88" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E88" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="F88" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>GRIFERIAS</t>
-        </is>
-      </c>
-      <c r="C89" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="D89" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E89" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="F89" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>INODOROS</t>
-        </is>
-      </c>
-      <c r="C90" s="2" t="n">
-        <v>2100</v>
-      </c>
-      <c r="D90" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E90" s="2" t="n">
-        <v>2100</v>
-      </c>
-      <c r="F90" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>LAVABOS</t>
-        </is>
-      </c>
-      <c r="C91" s="2" t="n">
-        <v>750</v>
-      </c>
-      <c r="D91" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E91" s="2" t="n">
-        <v>750</v>
-      </c>
-      <c r="F91" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="C92" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D92" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E92" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F92" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>NO RESURTIBLES</t>
-        </is>
-      </c>
-      <c r="C93" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="D93" s="2" t="n">
-        <v>9.58</v>
-      </c>
-      <c r="E93" s="2" t="n">
-        <v>640.67</v>
-      </c>
-      <c r="F93" s="5" t="n">
-        <v>0.01473279507881584</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C94" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D94" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E94" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F94" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>PANELES DECORATIVOS</t>
-        </is>
-      </c>
-      <c r="C95" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="D95" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E95" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="F95" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>PANELES PU</t>
-        </is>
-      </c>
-      <c r="C96" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="D96" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E96" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="F96" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>PANELES PVC</t>
-        </is>
-      </c>
-      <c r="C97" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="D97" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E97" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="F97" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>PIEDRA SINTERIZADA</t>
-        </is>
-      </c>
-      <c r="C98" s="2" t="n">
-        <v>1505.12</v>
-      </c>
-      <c r="D98" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E98" s="2" t="n">
-        <v>1505.12</v>
-      </c>
-      <c r="F98" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C99" s="2" t="n">
-        <v>38417.17</v>
-      </c>
-      <c r="D99" s="2" t="n">
-        <v>233.38</v>
-      </c>
-      <c r="E99" s="2" t="n">
-        <v>38183.79</v>
-      </c>
-      <c r="F99" s="5" t="n">
-        <v>0.006074887869148092</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>PUERTAS DE SEGURIDAD</t>
-        </is>
-      </c>
-      <c r="C100" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="D100" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E100" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="F100" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>SAL SOLUBLE</t>
-        </is>
-      </c>
-      <c r="C101" s="2" t="n">
-        <v>4130</v>
-      </c>
-      <c r="D101" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E101" s="2" t="n">
-        <v>4130</v>
-      </c>
-      <c r="F101" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>240X120 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C102" s="2" t="n">
-        <v>344.284604629486</v>
-      </c>
-      <c r="D102" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E102" s="2" t="n">
-        <v>344.284604629486</v>
-      </c>
-      <c r="F102" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>240X80 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C103" s="2" t="n">
-        <v>3120.1145</v>
-      </c>
-      <c r="D103" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E103" s="2" t="n">
-        <v>3120.1145</v>
-      </c>
-      <c r="F103" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>FREGADEROS DE COCINA</t>
-        </is>
-      </c>
-      <c r="C104" s="2" t="n">
-        <v>250.631825420901</v>
-      </c>
-      <c r="D104" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E104" s="2" t="n">
-        <v>250.631825420901</v>
-      </c>
-      <c r="F104" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>GRANITO</t>
-        </is>
-      </c>
-      <c r="C105" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="D105" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E105" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="F105" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>GRIFERIAS</t>
-        </is>
-      </c>
-      <c r="C106" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="D106" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E106" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="F106" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>INODOROS</t>
-        </is>
-      </c>
-      <c r="C107" s="2" t="n">
-        <v>560</v>
-      </c>
-      <c r="D107" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E107" s="2" t="n">
-        <v>560</v>
-      </c>
-      <c r="F107" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>LAVABOS</t>
-        </is>
-      </c>
-      <c r="C108" s="2" t="n">
-        <v>625</v>
-      </c>
-      <c r="D108" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E108" s="2" t="n">
-        <v>625</v>
-      </c>
-      <c r="F108" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="C109" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D109" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E109" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F109" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>NO RESURTIBLES</t>
-        </is>
-      </c>
-      <c r="C110" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="D110" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E110" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="F110" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C111" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D111" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E111" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F111" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>PANELES DECORATIVOS</t>
-        </is>
-      </c>
-      <c r="C112" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="D112" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E112" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="F112" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>PANELES PU</t>
-        </is>
-      </c>
-      <c r="C113" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="D113" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E113" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="F113" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>PANELES PVC</t>
-        </is>
-      </c>
-      <c r="C114" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="D114" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E114" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="F114" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>PIEDRA SINTERIZADA</t>
-        </is>
-      </c>
-      <c r="C115" s="2" t="n">
-        <v>1638</v>
-      </c>
-      <c r="D115" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E115" s="2" t="n">
-        <v>1638</v>
-      </c>
-      <c r="F115" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C116" s="2" t="n">
-        <v>13061.58</v>
-      </c>
-      <c r="D116" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E116" s="2" t="n">
-        <v>13061.58</v>
-      </c>
-      <c r="F116" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>PUERTAS DE SEGURIDAD</t>
-        </is>
-      </c>
-      <c r="C117" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="D117" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E117" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="F117" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>SAL SOLUBLE</t>
-        </is>
-      </c>
-      <c r="C118" s="2" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D118" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E118" s="2" t="n">
-        <v>1200</v>
-      </c>
-      <c r="F118" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>OFICINA-CATAECSA</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C119" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D119" s="2" t="n">
-        <v>605.48</v>
-      </c>
-      <c r="E119" s="2" t="n">
-        <v>-605.48</v>
-      </c>
-      <c r="F119" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>OFICINA-CATAECSA</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C120" s="2" t="n">
-        <v>17500</v>
-      </c>
-      <c r="D120" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E120" s="2" t="n">
-        <v>17500</v>
-      </c>
-      <c r="F120" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>240X120 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C121" s="2" t="n">
-        <v>1041.16</v>
-      </c>
-      <c r="D121" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E121" s="2" t="n">
-        <v>1041.16</v>
-      </c>
-      <c r="F121" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>240X80 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C122" s="2" t="n">
-        <v>8668.91</v>
-      </c>
-      <c r="D122" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E122" s="2" t="n">
-        <v>8668.91</v>
-      </c>
-      <c r="F122" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>FREGADEROS DE COCINA</t>
-        </is>
-      </c>
-      <c r="C123" s="2" t="n">
-        <v>372.993863046034</v>
-      </c>
-      <c r="D123" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E123" s="2" t="n">
-        <v>372.993863046034</v>
-      </c>
-      <c r="F123" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>GRANITO</t>
-        </is>
-      </c>
-      <c r="C124" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="D124" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E124" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="F124" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>GRIFERIAS</t>
-        </is>
-      </c>
-      <c r="C125" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="D125" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E125" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="F125" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>INODOROS</t>
-        </is>
-      </c>
-      <c r="C126" s="2" t="n">
-        <v>800</v>
-      </c>
-      <c r="D126" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E126" s="2" t="n">
-        <v>800</v>
-      </c>
-      <c r="F126" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>LAVABOS</t>
-        </is>
-      </c>
-      <c r="C127" s="2" t="n">
-        <v>625</v>
-      </c>
-      <c r="D127" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E127" s="2" t="n">
-        <v>625</v>
-      </c>
-      <c r="F127" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="C128" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D128" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E128" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F128" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>NO RESURTIBLES</t>
-        </is>
-      </c>
-      <c r="C129" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="D129" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E129" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="F129" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C130" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D130" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E130" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F130" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>PANELES DECORATIVOS</t>
-        </is>
-      </c>
-      <c r="C131" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="D131" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E131" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="F131" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>PANELES PU</t>
-        </is>
-      </c>
-      <c r="C132" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="D132" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E132" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="F132" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>PANELES PVC</t>
-        </is>
-      </c>
-      <c r="C133" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="D133" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E133" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="F133" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>PIEDRA SINTERIZADA</t>
-        </is>
-      </c>
-      <c r="C134" s="2" t="n">
-        <v>2501.01</v>
-      </c>
-      <c r="D134" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E134" s="2" t="n">
-        <v>2501.01</v>
-      </c>
-      <c r="F134" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C135" s="2" t="n">
-        <v>28209.84</v>
-      </c>
-      <c r="D135" s="2" t="n">
-        <v>-22.68</v>
-      </c>
-      <c r="E135" s="2" t="n">
-        <v>28232.52</v>
-      </c>
-      <c r="F135" s="5" t="n">
-        <v>-0.0008039747832671153</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>PUERTAS DE SEGURIDAD</t>
-        </is>
-      </c>
-      <c r="C136" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="D136" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E136" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="F136" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>SAL SOLUBLE</t>
-        </is>
-      </c>
-      <c r="C137" s="2" t="n">
-        <v>2300</v>
-      </c>
-      <c r="D137" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E137" s="2" t="n">
-        <v>2300</v>
-      </c>
-      <c r="F137" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="B138" s="6" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="C138" s="2" t="n">
-        <v>422464.7705625342</v>
-      </c>
-      <c r="D138" s="2" t="n">
-        <v>8919.789999999999</v>
-      </c>
-      <c r="E138" s="2" t="n">
-        <v>413544.9805625342</v>
-      </c>
-      <c r="F138" s="5" t="n">
-        <v>0.0211136895228514</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización automática 2025-06-05 11:18:26
</commit_message>
<xml_diff>
--- a/data/STROBEL CORDERO MARIA ELISABETH.xlsx
+++ b/data/STROBEL CORDERO MARIA ELISABETH.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="VENTAS POR GRUPO" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="VENTA MENSUAL" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="CUMPLIMIENTO MENSUAL" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -58,7 +59,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -68,6 +69,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -20328,4 +20333,3346 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F138"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="34" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="28" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ASESOR</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>GRUPO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>PRESUPUESTO</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>POR CUMPLIR</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>CUMPLIMIENTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>240X120 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>260.285000070615</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>260.285000070615</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>240X80 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>3120.1145</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>3120.1145</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>FREGADEROS DE COCINA</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>646.361575487259</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>646.361575487259</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>GRANITO</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>GRIFERIAS</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>INODOROS</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1260</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>1260</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>LAVABOS</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>NO RESURTIBLES</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>PANELES DECORATIVOS</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>PANELES PU</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PANELES PVC</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>PIEDRA SINTERIZADA</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>527.03</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>527.03</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>18798.61</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>18798.61</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>PUERTAS DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SAL SOLUBLE</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>1600</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>1600</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>240X120 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>5820</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>1669.25</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>4150.75</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <v>0.2868127147766323</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>240X80 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>13728</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>13728</v>
+      </c>
+      <c r="F20" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>FREGADEROS DE COCINA</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>646</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>128.74</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>517.26</v>
+      </c>
+      <c r="F21" s="5" t="n">
+        <v>0.1992879256965945</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>GRANITO</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>GRIFERIAS</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>INODOROS</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>2100</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>2100</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>LAVABOS</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F25" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F26" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>NO RESURTIBLES</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>1300.5</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>1300.5</v>
+      </c>
+      <c r="F27" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>PANELES DECORATIVOS</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F29" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>PANELES PU</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="F30" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>PANELES PVC</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>966</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>966</v>
+      </c>
+      <c r="F31" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>PIEDRA SINTERIZADA</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>15690</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>2568.3</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>13121.7</v>
+      </c>
+      <c r="F32" s="5" t="n">
+        <v>0.1636902485659656</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>45745.689</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>346.47</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>45399.219</v>
+      </c>
+      <c r="F33" s="5" t="n">
+        <v>0.007573828432226697</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>PUERTAS DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>1142</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>1142</v>
+      </c>
+      <c r="F34" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SAL SOLUBLE</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>1600</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>1600</v>
+      </c>
+      <c r="F35" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>240X80 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F36" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>FREGADEROS DE COCINA</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>250.631825420901</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>250.631825420901</v>
+      </c>
+      <c r="F37" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>GRANITO</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="F38" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>GRIFERIAS</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="F39" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>INODOROS</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>800</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>800</v>
+      </c>
+      <c r="F40" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>LAVABOS</t>
+        </is>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>500</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>500</v>
+      </c>
+      <c r="F41" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F42" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>NO RESURTIBLES</t>
+        </is>
+      </c>
+      <c r="C43" s="2" t="n">
+        <v>325.13</v>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>325.13</v>
+      </c>
+      <c r="F43" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>851.4299999999999</v>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>-851.4299999999999</v>
+      </c>
+      <c r="F44" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>PANELES DECORATIVOS</t>
+        </is>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F45" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>PANELES PU</t>
+        </is>
+      </c>
+      <c r="C46" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="F46" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>PANELES PVC</t>
+        </is>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="D47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="F47" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C48" s="2" t="n">
+        <v>7774.1</v>
+      </c>
+      <c r="D48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" s="2" t="n">
+        <v>7774.1</v>
+      </c>
+      <c r="F48" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>PUERTAS DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="C49" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="D49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="F49" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>SAL SOLUBLE</t>
+        </is>
+      </c>
+      <c r="C50" s="2" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="2" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F50" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>240X120 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C51" s="2" t="n">
+        <v>9970.34304517915</v>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="2" t="n">
+        <v>9970.34304517915</v>
+      </c>
+      <c r="F51" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>240X80 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C52" s="2" t="n">
+        <v>27457.0076</v>
+      </c>
+      <c r="D52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="2" t="n">
+        <v>27457.0076</v>
+      </c>
+      <c r="F52" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>FREGADEROS DE COCINA</t>
+        </is>
+      </c>
+      <c r="C53" s="2" t="n">
+        <v>1003</v>
+      </c>
+      <c r="D53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" s="2" t="n">
+        <v>1003</v>
+      </c>
+      <c r="F53" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>GRANITO</t>
+        </is>
+      </c>
+      <c r="C54" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="D54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="F54" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>GRIFERIAS</t>
+        </is>
+      </c>
+      <c r="C55" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="D55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="F55" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>INODOROS</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="n">
+        <v>1400</v>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="2" t="n">
+        <v>1400</v>
+      </c>
+      <c r="F56" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>LAVABOS</t>
+        </is>
+      </c>
+      <c r="C57" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F57" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F58" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>NO RESURTIBLES</t>
+        </is>
+      </c>
+      <c r="C59" s="2" t="n">
+        <v>1300.5</v>
+      </c>
+      <c r="D59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" s="2" t="n">
+        <v>1300.5</v>
+      </c>
+      <c r="F59" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>PANELES DECORATIVOS</t>
+        </is>
+      </c>
+      <c r="C61" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="D61" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F61" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>PANELES PU</t>
+        </is>
+      </c>
+      <c r="C62" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="D62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="F62" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>PANELES PVC</t>
+        </is>
+      </c>
+      <c r="C63" s="2" t="n">
+        <v>966</v>
+      </c>
+      <c r="D63" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" s="2" t="n">
+        <v>966</v>
+      </c>
+      <c r="F63" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>PIEDRA SINTERIZADA</t>
+        </is>
+      </c>
+      <c r="C64" s="2" t="n">
+        <v>13500</v>
+      </c>
+      <c r="D64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2" t="n">
+        <v>13500</v>
+      </c>
+      <c r="F64" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C65" s="2" t="n">
+        <v>32741.45</v>
+      </c>
+      <c r="D65" s="2" t="n">
+        <v>2529.84</v>
+      </c>
+      <c r="E65" s="2" t="n">
+        <v>30211.61</v>
+      </c>
+      <c r="F65" s="5" t="n">
+        <v>0.07726719494707779</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>PUERTAS DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="n">
+        <v>684</v>
+      </c>
+      <c r="D66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" s="2" t="n">
+        <v>684</v>
+      </c>
+      <c r="F66" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>SAL SOLUBLE</t>
+        </is>
+      </c>
+      <c r="C67" s="2" t="n">
+        <v>3200</v>
+      </c>
+      <c r="D67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2" t="n">
+        <v>3200</v>
+      </c>
+      <c r="F67" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>240X120 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C68" s="2" t="n">
+        <v>782.465010521559</v>
+      </c>
+      <c r="D68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" s="2" t="n">
+        <v>782.465010521559</v>
+      </c>
+      <c r="F68" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>240X80 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C69" s="2" t="n">
+        <v>4168.07156573679</v>
+      </c>
+      <c r="D69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" s="2" t="n">
+        <v>4168.07156573679</v>
+      </c>
+      <c r="F69" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>FREGADEROS DE COCINA</t>
+        </is>
+      </c>
+      <c r="C70" s="2" t="n">
+        <v>513.831046659336</v>
+      </c>
+      <c r="D70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2" t="n">
+        <v>513.831046659336</v>
+      </c>
+      <c r="F70" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>GRANITO</t>
+        </is>
+      </c>
+      <c r="C71" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="D71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="F71" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>GRIFERIAS</t>
+        </is>
+      </c>
+      <c r="C72" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="D72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="F72" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>INODOROS</t>
+        </is>
+      </c>
+      <c r="C73" s="2" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" s="2" t="n">
+        <v>1800</v>
+      </c>
+      <c r="F73" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>LAVABOS</t>
+        </is>
+      </c>
+      <c r="C74" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="D74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="F74" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="C75" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F75" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>NO RESURTIBLES</t>
+        </is>
+      </c>
+      <c r="C76" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="D76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="F76" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>PANELES DECORATIVOS</t>
+        </is>
+      </c>
+      <c r="C78" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="D78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F78" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>PANELES PU</t>
+        </is>
+      </c>
+      <c r="C79" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="D79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="F79" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>PANELES PVC</t>
+        </is>
+      </c>
+      <c r="C80" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="F80" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>PIEDRA SINTERIZADA</t>
+        </is>
+      </c>
+      <c r="C81" s="2" t="n">
+        <v>7465</v>
+      </c>
+      <c r="D81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" s="2" t="n">
+        <v>7465</v>
+      </c>
+      <c r="F81" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C82" s="2" t="n">
+        <v>29532.44</v>
+      </c>
+      <c r="D82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E82" s="2" t="n">
+        <v>29532.44</v>
+      </c>
+      <c r="F82" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>PUERTAS DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="C83" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="D83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="F83" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>SAL SOLUBLE</t>
+        </is>
+      </c>
+      <c r="C84" s="2" t="n">
+        <v>2800</v>
+      </c>
+      <c r="D84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" s="2" t="n">
+        <v>2800</v>
+      </c>
+      <c r="F84" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>240X120 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C85" s="2" t="n">
+        <v>672.340305337043</v>
+      </c>
+      <c r="D85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" s="2" t="n">
+        <v>672.340305337043</v>
+      </c>
+      <c r="F85" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>240X80 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C86" s="2" t="n">
+        <v>4992.1832</v>
+      </c>
+      <c r="D86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" s="2" t="n">
+        <v>4992.1832</v>
+      </c>
+      <c r="F86" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>FREGADEROS DE COCINA</t>
+        </is>
+      </c>
+      <c r="C87" s="2" t="n">
+        <v>142.502095025027</v>
+      </c>
+      <c r="D87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E87" s="2" t="n">
+        <v>142.502095025027</v>
+      </c>
+      <c r="F87" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>GRANITO</t>
+        </is>
+      </c>
+      <c r="C88" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="D88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E88" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="F88" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>GRIFERIAS</t>
+        </is>
+      </c>
+      <c r="C89" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="D89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E89" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="F89" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>INODOROS</t>
+        </is>
+      </c>
+      <c r="C90" s="2" t="n">
+        <v>2100</v>
+      </c>
+      <c r="D90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E90" s="2" t="n">
+        <v>2100</v>
+      </c>
+      <c r="F90" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>LAVABOS</t>
+        </is>
+      </c>
+      <c r="C91" s="2" t="n">
+        <v>750</v>
+      </c>
+      <c r="D91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E91" s="2" t="n">
+        <v>750</v>
+      </c>
+      <c r="F91" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="C92" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F92" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>NO RESURTIBLES</t>
+        </is>
+      </c>
+      <c r="C93" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="D93" s="2" t="n">
+        <v>9.58</v>
+      </c>
+      <c r="E93" s="2" t="n">
+        <v>640.67</v>
+      </c>
+      <c r="F93" s="5" t="n">
+        <v>0.01473279507881584</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F94" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>PANELES DECORATIVOS</t>
+        </is>
+      </c>
+      <c r="C95" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="D95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E95" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F95" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>PANELES PU</t>
+        </is>
+      </c>
+      <c r="C96" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="D96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E96" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="F96" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>PANELES PVC</t>
+        </is>
+      </c>
+      <c r="C97" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="D97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E97" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="F97" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>PIEDRA SINTERIZADA</t>
+        </is>
+      </c>
+      <c r="C98" s="2" t="n">
+        <v>1505.12</v>
+      </c>
+      <c r="D98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E98" s="2" t="n">
+        <v>1505.12</v>
+      </c>
+      <c r="F98" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C99" s="2" t="n">
+        <v>38417.17</v>
+      </c>
+      <c r="D99" s="2" t="n">
+        <v>233.38</v>
+      </c>
+      <c r="E99" s="2" t="n">
+        <v>38183.79</v>
+      </c>
+      <c r="F99" s="5" t="n">
+        <v>0.006074887869148092</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>PUERTAS DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="C100" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="D100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E100" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="F100" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>SAL SOLUBLE</t>
+        </is>
+      </c>
+      <c r="C101" s="2" t="n">
+        <v>4130</v>
+      </c>
+      <c r="D101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E101" s="2" t="n">
+        <v>4130</v>
+      </c>
+      <c r="F101" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>240X120 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C102" s="2" t="n">
+        <v>344.284604629486</v>
+      </c>
+      <c r="D102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E102" s="2" t="n">
+        <v>344.284604629486</v>
+      </c>
+      <c r="F102" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>240X80 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C103" s="2" t="n">
+        <v>3120.1145</v>
+      </c>
+      <c r="D103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E103" s="2" t="n">
+        <v>3120.1145</v>
+      </c>
+      <c r="F103" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>FREGADEROS DE COCINA</t>
+        </is>
+      </c>
+      <c r="C104" s="2" t="n">
+        <v>250.631825420901</v>
+      </c>
+      <c r="D104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E104" s="2" t="n">
+        <v>250.631825420901</v>
+      </c>
+      <c r="F104" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>GRANITO</t>
+        </is>
+      </c>
+      <c r="C105" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="D105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E105" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="F105" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>GRIFERIAS</t>
+        </is>
+      </c>
+      <c r="C106" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="D106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E106" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="F106" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>INODOROS</t>
+        </is>
+      </c>
+      <c r="C107" s="2" t="n">
+        <v>560</v>
+      </c>
+      <c r="D107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E107" s="2" t="n">
+        <v>560</v>
+      </c>
+      <c r="F107" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>LAVABOS</t>
+        </is>
+      </c>
+      <c r="C108" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="D108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E108" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="F108" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="C109" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E109" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F109" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>NO RESURTIBLES</t>
+        </is>
+      </c>
+      <c r="C110" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="D110" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E110" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="F110" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F111" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>PANELES DECORATIVOS</t>
+        </is>
+      </c>
+      <c r="C112" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="D112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E112" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F112" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>PANELES PU</t>
+        </is>
+      </c>
+      <c r="C113" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="D113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E113" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="F113" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>PANELES PVC</t>
+        </is>
+      </c>
+      <c r="C114" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="D114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E114" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="F114" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>PIEDRA SINTERIZADA</t>
+        </is>
+      </c>
+      <c r="C115" s="2" t="n">
+        <v>1638</v>
+      </c>
+      <c r="D115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E115" s="2" t="n">
+        <v>1638</v>
+      </c>
+      <c r="F115" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C116" s="2" t="n">
+        <v>13061.58</v>
+      </c>
+      <c r="D116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E116" s="2" t="n">
+        <v>13061.58</v>
+      </c>
+      <c r="F116" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>PUERTAS DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="C117" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="D117" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E117" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="F117" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>SAL SOLUBLE</t>
+        </is>
+      </c>
+      <c r="C118" s="2" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E118" s="2" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F118" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D119" s="2" t="n">
+        <v>605.48</v>
+      </c>
+      <c r="E119" s="2" t="n">
+        <v>-605.48</v>
+      </c>
+      <c r="F119" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C120" s="2" t="n">
+        <v>17500</v>
+      </c>
+      <c r="D120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E120" s="2" t="n">
+        <v>17500</v>
+      </c>
+      <c r="F120" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>240X120 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C121" s="2" t="n">
+        <v>1041.16</v>
+      </c>
+      <c r="D121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E121" s="2" t="n">
+        <v>1041.16</v>
+      </c>
+      <c r="F121" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>240X80 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C122" s="2" t="n">
+        <v>8668.91</v>
+      </c>
+      <c r="D122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E122" s="2" t="n">
+        <v>8668.91</v>
+      </c>
+      <c r="F122" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>FREGADEROS DE COCINA</t>
+        </is>
+      </c>
+      <c r="C123" s="2" t="n">
+        <v>372.993863046034</v>
+      </c>
+      <c r="D123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E123" s="2" t="n">
+        <v>372.993863046034</v>
+      </c>
+      <c r="F123" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>GRANITO</t>
+        </is>
+      </c>
+      <c r="C124" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="D124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E124" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="F124" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>GRIFERIAS</t>
+        </is>
+      </c>
+      <c r="C125" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="D125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E125" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="F125" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>INODOROS</t>
+        </is>
+      </c>
+      <c r="C126" s="2" t="n">
+        <v>800</v>
+      </c>
+      <c r="D126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E126" s="2" t="n">
+        <v>800</v>
+      </c>
+      <c r="F126" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>LAVABOS</t>
+        </is>
+      </c>
+      <c r="C127" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="D127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E127" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="F127" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="C128" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E128" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F128" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>NO RESURTIBLES</t>
+        </is>
+      </c>
+      <c r="C129" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="D129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E129" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="F129" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F130" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>PANELES DECORATIVOS</t>
+        </is>
+      </c>
+      <c r="C131" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="D131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E131" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F131" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>PANELES PU</t>
+        </is>
+      </c>
+      <c r="C132" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="D132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E132" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="F132" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>PANELES PVC</t>
+        </is>
+      </c>
+      <c r="C133" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="D133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E133" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="F133" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>PIEDRA SINTERIZADA</t>
+        </is>
+      </c>
+      <c r="C134" s="2" t="n">
+        <v>2501.01</v>
+      </c>
+      <c r="D134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E134" s="2" t="n">
+        <v>2501.01</v>
+      </c>
+      <c r="F134" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C135" s="2" t="n">
+        <v>28209.84</v>
+      </c>
+      <c r="D135" s="2" t="n">
+        <v>-22.68</v>
+      </c>
+      <c r="E135" s="2" t="n">
+        <v>28232.52</v>
+      </c>
+      <c r="F135" s="5" t="n">
+        <v>-0.0008039747832671153</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>PUERTAS DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="C136" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="D136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E136" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="F136" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>SAL SOLUBLE</t>
+        </is>
+      </c>
+      <c r="C137" s="2" t="n">
+        <v>2300</v>
+      </c>
+      <c r="D137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E137" s="2" t="n">
+        <v>2300</v>
+      </c>
+      <c r="F137" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="B138" s="6" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="C138" s="2" t="n">
+        <v>422464.7705625342</v>
+      </c>
+      <c r="D138" s="2" t="n">
+        <v>8919.789999999999</v>
+      </c>
+      <c r="E138" s="2" t="n">
+        <v>413544.9805625342</v>
+      </c>
+      <c r="F138" s="5" t="n">
+        <v>0.0211136895228514</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización automática 2025-06-05 11:40:36
</commit_message>
<xml_diff>
--- a/data/STROBEL CORDERO MARIA ELISABETH.xlsx
+++ b/data/STROBEL CORDERO MARIA ELISABETH.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="VENTAS POR GRUPO" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="VENTA MENSUAL" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="CUMPLIMIENTO MENSUAL" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -59,7 +58,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -69,10 +68,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -20333,3346 +20328,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F138"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="34" customWidth="1" min="1" max="1"/>
-    <col width="22" customWidth="1" min="2" max="2"/>
-    <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
-    <col width="28" customWidth="1" min="6" max="6"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ASESOR</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>GRUPO</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>PRESUPUESTO</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>VENTA</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>POR CUMPLIR</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>CUMPLIMIENTO</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>240X120 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>260.285000070615</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>260.285000070615</v>
-      </c>
-      <c r="F2" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>240X80 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>3120.1145</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>3120.1145</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>FREGADEROS DE COCINA</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>646.361575487259</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>646.361575487259</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>GRANITO</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>GRIFERIAS</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="F6" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>INODOROS</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>1260</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>1260</v>
-      </c>
-      <c r="F7" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>LAVABOS</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>625</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>625</v>
-      </c>
-      <c r="F8" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F9" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>NO RESURTIBLES</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="F10" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>PANELES DECORATIVOS</t>
-        </is>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="F12" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>PANELES PU</t>
-        </is>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="F13" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>PANELES PVC</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="F14" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>PIEDRA SINTERIZADA</t>
-        </is>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>527.03</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>527.03</v>
-      </c>
-      <c r="F15" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C16" s="2" t="n">
-        <v>18798.61</v>
-      </c>
-      <c r="D16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>18798.61</v>
-      </c>
-      <c r="F16" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>PUERTAS DE SEGURIDAD</t>
-        </is>
-      </c>
-      <c r="C17" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="F17" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>SAL SOLUBLE</t>
-        </is>
-      </c>
-      <c r="C18" s="2" t="n">
-        <v>1600</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>1600</v>
-      </c>
-      <c r="F18" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>240X120 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C19" s="2" t="n">
-        <v>5820</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>1669.25</v>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>4150.75</v>
-      </c>
-      <c r="F19" s="5" t="n">
-        <v>0.2868127147766323</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>240X80 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C20" s="2" t="n">
-        <v>13728</v>
-      </c>
-      <c r="D20" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>13728</v>
-      </c>
-      <c r="F20" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>FREGADEROS DE COCINA</t>
-        </is>
-      </c>
-      <c r="C21" s="2" t="n">
-        <v>646</v>
-      </c>
-      <c r="D21" s="2" t="n">
-        <v>128.74</v>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>517.26</v>
-      </c>
-      <c r="F21" s="5" t="n">
-        <v>0.1992879256965945</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>GRANITO</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="D22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="F22" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>GRIFERIAS</t>
-        </is>
-      </c>
-      <c r="C23" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="D23" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="F23" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>INODOROS</t>
-        </is>
-      </c>
-      <c r="C24" s="2" t="n">
-        <v>2100</v>
-      </c>
-      <c r="D24" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>2100</v>
-      </c>
-      <c r="F24" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>LAVABOS</t>
-        </is>
-      </c>
-      <c r="C25" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D25" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F25" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="C26" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F26" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>NO RESURTIBLES</t>
-        </is>
-      </c>
-      <c r="C27" s="2" t="n">
-        <v>1300.5</v>
-      </c>
-      <c r="D27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>1300.5</v>
-      </c>
-      <c r="F27" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>PANELES DECORATIVOS</t>
-        </is>
-      </c>
-      <c r="C29" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="D29" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="F29" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>PANELES PU</t>
-        </is>
-      </c>
-      <c r="C30" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="F30" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>PANELES PVC</t>
-        </is>
-      </c>
-      <c r="C31" s="2" t="n">
-        <v>966</v>
-      </c>
-      <c r="D31" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2" t="n">
-        <v>966</v>
-      </c>
-      <c r="F31" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>PIEDRA SINTERIZADA</t>
-        </is>
-      </c>
-      <c r="C32" s="2" t="n">
-        <v>15690</v>
-      </c>
-      <c r="D32" s="2" t="n">
-        <v>2568.3</v>
-      </c>
-      <c r="E32" s="2" t="n">
-        <v>13121.7</v>
-      </c>
-      <c r="F32" s="5" t="n">
-        <v>0.1636902485659656</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C33" s="2" t="n">
-        <v>45745.689</v>
-      </c>
-      <c r="D33" s="2" t="n">
-        <v>346.47</v>
-      </c>
-      <c r="E33" s="2" t="n">
-        <v>45399.219</v>
-      </c>
-      <c r="F33" s="5" t="n">
-        <v>0.007573828432226697</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>PUERTAS DE SEGURIDAD</t>
-        </is>
-      </c>
-      <c r="C34" s="2" t="n">
-        <v>1142</v>
-      </c>
-      <c r="D34" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" s="2" t="n">
-        <v>1142</v>
-      </c>
-      <c r="F34" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>CASTRO ALCIVAR EDA MARIA</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>SAL SOLUBLE</t>
-        </is>
-      </c>
-      <c r="C35" s="2" t="n">
-        <v>1600</v>
-      </c>
-      <c r="D35" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" s="2" t="n">
-        <v>1600</v>
-      </c>
-      <c r="F35" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>240X80 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C36" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D36" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F36" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>FREGADEROS DE COCINA</t>
-        </is>
-      </c>
-      <c r="C37" s="2" t="n">
-        <v>250.631825420901</v>
-      </c>
-      <c r="D37" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" s="2" t="n">
-        <v>250.631825420901</v>
-      </c>
-      <c r="F37" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>GRANITO</t>
-        </is>
-      </c>
-      <c r="C38" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="D38" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="F38" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>GRIFERIAS</t>
-        </is>
-      </c>
-      <c r="C39" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="D39" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="F39" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>INODOROS</t>
-        </is>
-      </c>
-      <c r="C40" s="2" t="n">
-        <v>800</v>
-      </c>
-      <c r="D40" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" s="2" t="n">
-        <v>800</v>
-      </c>
-      <c r="F40" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>LAVABOS</t>
-        </is>
-      </c>
-      <c r="C41" s="2" t="n">
-        <v>500</v>
-      </c>
-      <c r="D41" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" s="2" t="n">
-        <v>500</v>
-      </c>
-      <c r="F41" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="C42" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D42" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F42" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>NO RESURTIBLES</t>
-        </is>
-      </c>
-      <c r="C43" s="2" t="n">
-        <v>325.13</v>
-      </c>
-      <c r="D43" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" s="2" t="n">
-        <v>325.13</v>
-      </c>
-      <c r="F43" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C44" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" s="2" t="n">
-        <v>851.4299999999999</v>
-      </c>
-      <c r="E44" s="2" t="n">
-        <v>-851.4299999999999</v>
-      </c>
-      <c r="F44" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>PANELES DECORATIVOS</t>
-        </is>
-      </c>
-      <c r="C45" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="D45" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="F45" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>PANELES PU</t>
-        </is>
-      </c>
-      <c r="C46" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="D46" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E46" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="F46" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>PANELES PVC</t>
-        </is>
-      </c>
-      <c r="C47" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="D47" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="F47" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C48" s="2" t="n">
-        <v>7774.1</v>
-      </c>
-      <c r="D48" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E48" s="2" t="n">
-        <v>7774.1</v>
-      </c>
-      <c r="F48" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>PUERTAS DE SEGURIDAD</t>
-        </is>
-      </c>
-      <c r="C49" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="D49" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="F49" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>CHANDI ERAZO JOSUE</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>SAL SOLUBLE</t>
-        </is>
-      </c>
-      <c r="C50" s="2" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D50" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E50" s="2" t="n">
-        <v>1500</v>
-      </c>
-      <c r="F50" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>240X120 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C51" s="2" t="n">
-        <v>9970.34304517915</v>
-      </c>
-      <c r="D51" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" s="2" t="n">
-        <v>9970.34304517915</v>
-      </c>
-      <c r="F51" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>240X80 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C52" s="2" t="n">
-        <v>27457.0076</v>
-      </c>
-      <c r="D52" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E52" s="2" t="n">
-        <v>27457.0076</v>
-      </c>
-      <c r="F52" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>FREGADEROS DE COCINA</t>
-        </is>
-      </c>
-      <c r="C53" s="2" t="n">
-        <v>1003</v>
-      </c>
-      <c r="D53" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" s="2" t="n">
-        <v>1003</v>
-      </c>
-      <c r="F53" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>GRANITO</t>
-        </is>
-      </c>
-      <c r="C54" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="D54" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="F54" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>GRIFERIAS</t>
-        </is>
-      </c>
-      <c r="C55" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="D55" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E55" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="F55" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>INODOROS</t>
-        </is>
-      </c>
-      <c r="C56" s="2" t="n">
-        <v>1400</v>
-      </c>
-      <c r="D56" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E56" s="2" t="n">
-        <v>1400</v>
-      </c>
-      <c r="F56" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>LAVABOS</t>
-        </is>
-      </c>
-      <c r="C57" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D57" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E57" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F57" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="C58" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D58" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E58" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F58" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>NO RESURTIBLES</t>
-        </is>
-      </c>
-      <c r="C59" s="2" t="n">
-        <v>1300.5</v>
-      </c>
-      <c r="D59" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E59" s="2" t="n">
-        <v>1300.5</v>
-      </c>
-      <c r="F59" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C60" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D60" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E60" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F60" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>PANELES DECORATIVOS</t>
-        </is>
-      </c>
-      <c r="C61" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="D61" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E61" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="F61" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>PANELES PU</t>
-        </is>
-      </c>
-      <c r="C62" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="D62" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E62" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="F62" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>PANELES PVC</t>
-        </is>
-      </c>
-      <c r="C63" s="2" t="n">
-        <v>966</v>
-      </c>
-      <c r="D63" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E63" s="2" t="n">
-        <v>966</v>
-      </c>
-      <c r="F63" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>PIEDRA SINTERIZADA</t>
-        </is>
-      </c>
-      <c r="C64" s="2" t="n">
-        <v>13500</v>
-      </c>
-      <c r="D64" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E64" s="2" t="n">
-        <v>13500</v>
-      </c>
-      <c r="F64" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C65" s="2" t="n">
-        <v>32741.45</v>
-      </c>
-      <c r="D65" s="2" t="n">
-        <v>2529.84</v>
-      </c>
-      <c r="E65" s="2" t="n">
-        <v>30211.61</v>
-      </c>
-      <c r="F65" s="5" t="n">
-        <v>0.07726719494707779</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>PUERTAS DE SEGURIDAD</t>
-        </is>
-      </c>
-      <c r="C66" s="2" t="n">
-        <v>684</v>
-      </c>
-      <c r="D66" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E66" s="2" t="n">
-        <v>684</v>
-      </c>
-      <c r="F66" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>SAL SOLUBLE</t>
-        </is>
-      </c>
-      <c r="C67" s="2" t="n">
-        <v>3200</v>
-      </c>
-      <c r="D67" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E67" s="2" t="n">
-        <v>3200</v>
-      </c>
-      <c r="F67" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>240X120 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C68" s="2" t="n">
-        <v>782.465010521559</v>
-      </c>
-      <c r="D68" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E68" s="2" t="n">
-        <v>782.465010521559</v>
-      </c>
-      <c r="F68" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>240X80 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C69" s="2" t="n">
-        <v>4168.07156573679</v>
-      </c>
-      <c r="D69" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E69" s="2" t="n">
-        <v>4168.07156573679</v>
-      </c>
-      <c r="F69" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>FREGADEROS DE COCINA</t>
-        </is>
-      </c>
-      <c r="C70" s="2" t="n">
-        <v>513.831046659336</v>
-      </c>
-      <c r="D70" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E70" s="2" t="n">
-        <v>513.831046659336</v>
-      </c>
-      <c r="F70" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>GRANITO</t>
-        </is>
-      </c>
-      <c r="C71" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="D71" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E71" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="F71" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>GRIFERIAS</t>
-        </is>
-      </c>
-      <c r="C72" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="D72" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E72" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="F72" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>INODOROS</t>
-        </is>
-      </c>
-      <c r="C73" s="2" t="n">
-        <v>1800</v>
-      </c>
-      <c r="D73" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E73" s="2" t="n">
-        <v>1800</v>
-      </c>
-      <c r="F73" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>LAVABOS</t>
-        </is>
-      </c>
-      <c r="C74" s="2" t="n">
-        <v>625</v>
-      </c>
-      <c r="D74" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E74" s="2" t="n">
-        <v>625</v>
-      </c>
-      <c r="F74" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="C75" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D75" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E75" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F75" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>NO RESURTIBLES</t>
-        </is>
-      </c>
-      <c r="C76" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="D76" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E76" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="F76" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C77" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D77" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E77" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F77" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>PANELES DECORATIVOS</t>
-        </is>
-      </c>
-      <c r="C78" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="D78" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E78" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="F78" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>PANELES PU</t>
-        </is>
-      </c>
-      <c r="C79" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="D79" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E79" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="F79" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>PANELES PVC</t>
-        </is>
-      </c>
-      <c r="C80" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="D80" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E80" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="F80" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>PIEDRA SINTERIZADA</t>
-        </is>
-      </c>
-      <c r="C81" s="2" t="n">
-        <v>7465</v>
-      </c>
-      <c r="D81" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E81" s="2" t="n">
-        <v>7465</v>
-      </c>
-      <c r="F81" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C82" s="2" t="n">
-        <v>29532.44</v>
-      </c>
-      <c r="D82" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E82" s="2" t="n">
-        <v>29532.44</v>
-      </c>
-      <c r="F82" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>PUERTAS DE SEGURIDAD</t>
-        </is>
-      </c>
-      <c r="C83" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="D83" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E83" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="F83" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>SAL SOLUBLE</t>
-        </is>
-      </c>
-      <c r="C84" s="2" t="n">
-        <v>2800</v>
-      </c>
-      <c r="D84" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E84" s="2" t="n">
-        <v>2800</v>
-      </c>
-      <c r="F84" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>240X120 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C85" s="2" t="n">
-        <v>672.340305337043</v>
-      </c>
-      <c r="D85" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E85" s="2" t="n">
-        <v>672.340305337043</v>
-      </c>
-      <c r="F85" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>240X80 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C86" s="2" t="n">
-        <v>4992.1832</v>
-      </c>
-      <c r="D86" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E86" s="2" t="n">
-        <v>4992.1832</v>
-      </c>
-      <c r="F86" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>FREGADEROS DE COCINA</t>
-        </is>
-      </c>
-      <c r="C87" s="2" t="n">
-        <v>142.502095025027</v>
-      </c>
-      <c r="D87" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E87" s="2" t="n">
-        <v>142.502095025027</v>
-      </c>
-      <c r="F87" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>GRANITO</t>
-        </is>
-      </c>
-      <c r="C88" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="D88" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E88" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="F88" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>GRIFERIAS</t>
-        </is>
-      </c>
-      <c r="C89" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="D89" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E89" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="F89" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>INODOROS</t>
-        </is>
-      </c>
-      <c r="C90" s="2" t="n">
-        <v>2100</v>
-      </c>
-      <c r="D90" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E90" s="2" t="n">
-        <v>2100</v>
-      </c>
-      <c r="F90" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>LAVABOS</t>
-        </is>
-      </c>
-      <c r="C91" s="2" t="n">
-        <v>750</v>
-      </c>
-      <c r="D91" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E91" s="2" t="n">
-        <v>750</v>
-      </c>
-      <c r="F91" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="C92" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D92" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E92" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F92" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>NO RESURTIBLES</t>
-        </is>
-      </c>
-      <c r="C93" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="D93" s="2" t="n">
-        <v>9.58</v>
-      </c>
-      <c r="E93" s="2" t="n">
-        <v>640.67</v>
-      </c>
-      <c r="F93" s="5" t="n">
-        <v>0.01473279507881584</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C94" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D94" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E94" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F94" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>PANELES DECORATIVOS</t>
-        </is>
-      </c>
-      <c r="C95" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="D95" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E95" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="F95" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>PANELES PU</t>
-        </is>
-      </c>
-      <c r="C96" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="D96" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E96" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="F96" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>PANELES PVC</t>
-        </is>
-      </c>
-      <c r="C97" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="D97" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E97" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="F97" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>PIEDRA SINTERIZADA</t>
-        </is>
-      </c>
-      <c r="C98" s="2" t="n">
-        <v>1505.12</v>
-      </c>
-      <c r="D98" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E98" s="2" t="n">
-        <v>1505.12</v>
-      </c>
-      <c r="F98" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C99" s="2" t="n">
-        <v>38417.17</v>
-      </c>
-      <c r="D99" s="2" t="n">
-        <v>233.38</v>
-      </c>
-      <c r="E99" s="2" t="n">
-        <v>38183.79</v>
-      </c>
-      <c r="F99" s="5" t="n">
-        <v>0.006074887869148092</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>PUERTAS DE SEGURIDAD</t>
-        </is>
-      </c>
-      <c r="C100" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="D100" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E100" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="F100" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>SAL SOLUBLE</t>
-        </is>
-      </c>
-      <c r="C101" s="2" t="n">
-        <v>4130</v>
-      </c>
-      <c r="D101" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E101" s="2" t="n">
-        <v>4130</v>
-      </c>
-      <c r="F101" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>240X120 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C102" s="2" t="n">
-        <v>344.284604629486</v>
-      </c>
-      <c r="D102" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E102" s="2" t="n">
-        <v>344.284604629486</v>
-      </c>
-      <c r="F102" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>240X80 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C103" s="2" t="n">
-        <v>3120.1145</v>
-      </c>
-      <c r="D103" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E103" s="2" t="n">
-        <v>3120.1145</v>
-      </c>
-      <c r="F103" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>FREGADEROS DE COCINA</t>
-        </is>
-      </c>
-      <c r="C104" s="2" t="n">
-        <v>250.631825420901</v>
-      </c>
-      <c r="D104" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E104" s="2" t="n">
-        <v>250.631825420901</v>
-      </c>
-      <c r="F104" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>GRANITO</t>
-        </is>
-      </c>
-      <c r="C105" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="D105" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E105" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="F105" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>GRIFERIAS</t>
-        </is>
-      </c>
-      <c r="C106" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="D106" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E106" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="F106" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>INODOROS</t>
-        </is>
-      </c>
-      <c r="C107" s="2" t="n">
-        <v>560</v>
-      </c>
-      <c r="D107" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E107" s="2" t="n">
-        <v>560</v>
-      </c>
-      <c r="F107" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>LAVABOS</t>
-        </is>
-      </c>
-      <c r="C108" s="2" t="n">
-        <v>625</v>
-      </c>
-      <c r="D108" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E108" s="2" t="n">
-        <v>625</v>
-      </c>
-      <c r="F108" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="C109" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D109" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E109" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F109" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>NO RESURTIBLES</t>
-        </is>
-      </c>
-      <c r="C110" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="D110" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E110" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="F110" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C111" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D111" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E111" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F111" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>PANELES DECORATIVOS</t>
-        </is>
-      </c>
-      <c r="C112" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="D112" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E112" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="F112" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>PANELES PU</t>
-        </is>
-      </c>
-      <c r="C113" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="D113" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E113" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="F113" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>PANELES PVC</t>
-        </is>
-      </c>
-      <c r="C114" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="D114" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E114" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="F114" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>PIEDRA SINTERIZADA</t>
-        </is>
-      </c>
-      <c r="C115" s="2" t="n">
-        <v>1638</v>
-      </c>
-      <c r="D115" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E115" s="2" t="n">
-        <v>1638</v>
-      </c>
-      <c r="F115" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C116" s="2" t="n">
-        <v>13061.58</v>
-      </c>
-      <c r="D116" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E116" s="2" t="n">
-        <v>13061.58</v>
-      </c>
-      <c r="F116" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>PUERTAS DE SEGURIDAD</t>
-        </is>
-      </c>
-      <c r="C117" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="D117" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E117" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="F117" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>LOZANO MOLINA TITO</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>SAL SOLUBLE</t>
-        </is>
-      </c>
-      <c r="C118" s="2" t="n">
-        <v>1200</v>
-      </c>
-      <c r="D118" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E118" s="2" t="n">
-        <v>1200</v>
-      </c>
-      <c r="F118" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>OFICINA-CATAECSA</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C119" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D119" s="2" t="n">
-        <v>605.48</v>
-      </c>
-      <c r="E119" s="2" t="n">
-        <v>-605.48</v>
-      </c>
-      <c r="F119" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>OFICINA-CATAECSA</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C120" s="2" t="n">
-        <v>17500</v>
-      </c>
-      <c r="D120" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E120" s="2" t="n">
-        <v>17500</v>
-      </c>
-      <c r="F120" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>240X120 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C121" s="2" t="n">
-        <v>1041.16</v>
-      </c>
-      <c r="D121" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E121" s="2" t="n">
-        <v>1041.16</v>
-      </c>
-      <c r="F121" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>240X80 PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C122" s="2" t="n">
-        <v>8668.91</v>
-      </c>
-      <c r="D122" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E122" s="2" t="n">
-        <v>8668.91</v>
-      </c>
-      <c r="F122" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>FREGADEROS DE COCINA</t>
-        </is>
-      </c>
-      <c r="C123" s="2" t="n">
-        <v>372.993863046034</v>
-      </c>
-      <c r="D123" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E123" s="2" t="n">
-        <v>372.993863046034</v>
-      </c>
-      <c r="F123" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>GRANITO</t>
-        </is>
-      </c>
-      <c r="C124" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="D124" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E124" s="2" t="n">
-        <v>238.32</v>
-      </c>
-      <c r="F124" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>GRIFERIAS</t>
-        </is>
-      </c>
-      <c r="C125" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="D125" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E125" s="2" t="n">
-        <v>106.82</v>
-      </c>
-      <c r="F125" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>INODOROS</t>
-        </is>
-      </c>
-      <c r="C126" s="2" t="n">
-        <v>800</v>
-      </c>
-      <c r="D126" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E126" s="2" t="n">
-        <v>800</v>
-      </c>
-      <c r="F126" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>LAVABOS</t>
-        </is>
-      </c>
-      <c r="C127" s="2" t="n">
-        <v>625</v>
-      </c>
-      <c r="D127" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E127" s="2" t="n">
-        <v>625</v>
-      </c>
-      <c r="F127" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>LED</t>
-        </is>
-      </c>
-      <c r="C128" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="D128" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E128" s="2" t="n">
-        <v>300</v>
-      </c>
-      <c r="F128" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>NO RESURTIBLES</t>
-        </is>
-      </c>
-      <c r="C129" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="D129" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E129" s="2" t="n">
-        <v>650.25</v>
-      </c>
-      <c r="F129" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>OTROS</t>
-        </is>
-      </c>
-      <c r="C130" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D130" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E130" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F130" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>PANELES DECORATIVOS</t>
-        </is>
-      </c>
-      <c r="C131" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="D131" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E131" s="2" t="n">
-        <v>350</v>
-      </c>
-      <c r="F131" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>PANELES PU</t>
-        </is>
-      </c>
-      <c r="C132" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="D132" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E132" s="2" t="n">
-        <v>230</v>
-      </c>
-      <c r="F132" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>PANELES PVC</t>
-        </is>
-      </c>
-      <c r="C133" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="D133" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E133" s="2" t="n">
-        <v>483</v>
-      </c>
-      <c r="F133" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>PIEDRA SINTERIZADA</t>
-        </is>
-      </c>
-      <c r="C134" s="2" t="n">
-        <v>2501.01</v>
-      </c>
-      <c r="D134" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E134" s="2" t="n">
-        <v>2501.01</v>
-      </c>
-      <c r="F134" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>PORCELANATO</t>
-        </is>
-      </c>
-      <c r="C135" s="2" t="n">
-        <v>28209.84</v>
-      </c>
-      <c r="D135" s="2" t="n">
-        <v>-22.68</v>
-      </c>
-      <c r="E135" s="2" t="n">
-        <v>28232.52</v>
-      </c>
-      <c r="F135" s="5" t="n">
-        <v>-0.0008039747832671153</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>PUERTAS DE SEGURIDAD</t>
-        </is>
-      </c>
-      <c r="C136" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="D136" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E136" s="2" t="n">
-        <v>342</v>
-      </c>
-      <c r="F136" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>RIOS CARRION ANGEL BENIGNO</t>
-        </is>
-      </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>SAL SOLUBLE</t>
-        </is>
-      </c>
-      <c r="C137" s="2" t="n">
-        <v>2300</v>
-      </c>
-      <c r="D137" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E137" s="2" t="n">
-        <v>2300</v>
-      </c>
-      <c r="F137" s="5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="B138" s="6" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="C138" s="2" t="n">
-        <v>422464.7705625342</v>
-      </c>
-      <c r="D138" s="2" t="n">
-        <v>8919.789999999999</v>
-      </c>
-      <c r="E138" s="2" t="n">
-        <v>413544.9805625342</v>
-      </c>
-      <c r="F138" s="5" t="n">
-        <v>0.0211136895228514</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización automática 2025-06-05 11:55:08
</commit_message>
<xml_diff>
--- a/data/STROBEL CORDERO MARIA ELISABETH.xlsx
+++ b/data/STROBEL CORDERO MARIA ELISABETH.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="VENTAS POR GRUPO" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="VENTA MENSUAL" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="CUMPLIMIENTO MENSUAL" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -58,7 +59,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -68,6 +69,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -20328,4 +20333,3346 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F138"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="34" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="28" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ASESOR</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>GRUPO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>PRESUPUESTO</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>POR CUMPLIR</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>CUMPLIMIENTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>240X120 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>260.285000070615</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>260.285000070615</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>240X80 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>3120.1145</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>3120.1145</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>FREGADEROS DE COCINA</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>646.361575487259</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>646.361575487259</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>GRANITO</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>GRIFERIAS</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>INODOROS</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1260</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>1260</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>LAVABOS</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>NO RESURTIBLES</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>PANELES DECORATIVOS</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>PANELES PU</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PANELES PVC</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>PIEDRA SINTERIZADA</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>527.03</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>527.03</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>18798.61</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>18798.61</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>PUERTAS DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="F17" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ALMEIDA CUATIN JHONATHANN CARLOS</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SAL SOLUBLE</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>1600</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>1600</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>240X120 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>5820</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>1669.25</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>4150.75</v>
+      </c>
+      <c r="F19" s="5" t="n">
+        <v>0.2868127147766323</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>240X80 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>13728</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>13728</v>
+      </c>
+      <c r="F20" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>FREGADEROS DE COCINA</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>646</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>128.74</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>517.26</v>
+      </c>
+      <c r="F21" s="5" t="n">
+        <v>0.1992879256965945</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>GRANITO</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="F22" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>GRIFERIAS</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="D23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="F23" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>INODOROS</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>2100</v>
+      </c>
+      <c r="D24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>2100</v>
+      </c>
+      <c r="F24" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>LAVABOS</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F25" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F26" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>NO RESURTIBLES</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>1300.5</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>1300.5</v>
+      </c>
+      <c r="F27" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>PANELES DECORATIVOS</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F29" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>PANELES PU</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="F30" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>PANELES PVC</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>966</v>
+      </c>
+      <c r="D31" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>966</v>
+      </c>
+      <c r="F31" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>PIEDRA SINTERIZADA</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>15690</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>2568.3</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>13121.7</v>
+      </c>
+      <c r="F32" s="5" t="n">
+        <v>0.1636902485659656</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>45745.689</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>346.47</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>45399.219</v>
+      </c>
+      <c r="F33" s="5" t="n">
+        <v>0.007573828432226697</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>PUERTAS DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>1142</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>1142</v>
+      </c>
+      <c r="F34" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>CASTRO ALCIVAR EDA MARIA</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>SAL SOLUBLE</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>1600</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>1600</v>
+      </c>
+      <c r="F35" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>240X80 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F36" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>FREGADEROS DE COCINA</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>250.631825420901</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>250.631825420901</v>
+      </c>
+      <c r="F37" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>GRANITO</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="F38" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>GRIFERIAS</t>
+        </is>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="F39" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>INODOROS</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="n">
+        <v>800</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>800</v>
+      </c>
+      <c r="F40" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>LAVABOS</t>
+        </is>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>500</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>500</v>
+      </c>
+      <c r="F41" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F42" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>NO RESURTIBLES</t>
+        </is>
+      </c>
+      <c r="C43" s="2" t="n">
+        <v>325.13</v>
+      </c>
+      <c r="D43" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="n">
+        <v>325.13</v>
+      </c>
+      <c r="F43" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2" t="n">
+        <v>851.4299999999999</v>
+      </c>
+      <c r="E44" s="2" t="n">
+        <v>-851.4299999999999</v>
+      </c>
+      <c r="F44" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>PANELES DECORATIVOS</t>
+        </is>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="D45" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F45" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>PANELES PU</t>
+        </is>
+      </c>
+      <c r="C46" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="D46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="F46" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>PANELES PVC</t>
+        </is>
+      </c>
+      <c r="C47" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="D47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="F47" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C48" s="2" t="n">
+        <v>7774.1</v>
+      </c>
+      <c r="D48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" s="2" t="n">
+        <v>7774.1</v>
+      </c>
+      <c r="F48" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>PUERTAS DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="C49" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="D49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="F49" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>CHANDI ERAZO JOSUE</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>SAL SOLUBLE</t>
+        </is>
+      </c>
+      <c r="C50" s="2" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D50" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="2" t="n">
+        <v>1500</v>
+      </c>
+      <c r="F50" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>240X120 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C51" s="2" t="n">
+        <v>9970.34304517915</v>
+      </c>
+      <c r="D51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="2" t="n">
+        <v>9970.34304517915</v>
+      </c>
+      <c r="F51" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>240X80 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C52" s="2" t="n">
+        <v>27457.0076</v>
+      </c>
+      <c r="D52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="2" t="n">
+        <v>27457.0076</v>
+      </c>
+      <c r="F52" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>FREGADEROS DE COCINA</t>
+        </is>
+      </c>
+      <c r="C53" s="2" t="n">
+        <v>1003</v>
+      </c>
+      <c r="D53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" s="2" t="n">
+        <v>1003</v>
+      </c>
+      <c r="F53" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>GRANITO</t>
+        </is>
+      </c>
+      <c r="C54" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="D54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="F54" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>GRIFERIAS</t>
+        </is>
+      </c>
+      <c r="C55" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="D55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="F55" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>INODOROS</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="n">
+        <v>1400</v>
+      </c>
+      <c r="D56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="2" t="n">
+        <v>1400</v>
+      </c>
+      <c r="F56" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>LAVABOS</t>
+        </is>
+      </c>
+      <c r="C57" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F57" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F58" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>NO RESURTIBLES</t>
+        </is>
+      </c>
+      <c r="C59" s="2" t="n">
+        <v>1300.5</v>
+      </c>
+      <c r="D59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" s="2" t="n">
+        <v>1300.5</v>
+      </c>
+      <c r="F59" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F60" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>PANELES DECORATIVOS</t>
+        </is>
+      </c>
+      <c r="C61" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="D61" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F61" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>PANELES PU</t>
+        </is>
+      </c>
+      <c r="C62" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="D62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="F62" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>PANELES PVC</t>
+        </is>
+      </c>
+      <c r="C63" s="2" t="n">
+        <v>966</v>
+      </c>
+      <c r="D63" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" s="2" t="n">
+        <v>966</v>
+      </c>
+      <c r="F63" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>PIEDRA SINTERIZADA</t>
+        </is>
+      </c>
+      <c r="C64" s="2" t="n">
+        <v>13500</v>
+      </c>
+      <c r="D64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2" t="n">
+        <v>13500</v>
+      </c>
+      <c r="F64" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C65" s="2" t="n">
+        <v>32741.45</v>
+      </c>
+      <c r="D65" s="2" t="n">
+        <v>2529.84</v>
+      </c>
+      <c r="E65" s="2" t="n">
+        <v>30211.61</v>
+      </c>
+      <c r="F65" s="5" t="n">
+        <v>0.07726719494707779</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>PUERTAS DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="n">
+        <v>684</v>
+      </c>
+      <c r="D66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" s="2" t="n">
+        <v>684</v>
+      </c>
+      <c r="F66" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>GUERRERO FAREZ FABIAN MAURICIO</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>SAL SOLUBLE</t>
+        </is>
+      </c>
+      <c r="C67" s="2" t="n">
+        <v>3200</v>
+      </c>
+      <c r="D67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" s="2" t="n">
+        <v>3200</v>
+      </c>
+      <c r="F67" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>240X120 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C68" s="2" t="n">
+        <v>782.465010521559</v>
+      </c>
+      <c r="D68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" s="2" t="n">
+        <v>782.465010521559</v>
+      </c>
+      <c r="F68" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>240X80 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C69" s="2" t="n">
+        <v>4168.07156573679</v>
+      </c>
+      <c r="D69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" s="2" t="n">
+        <v>4168.07156573679</v>
+      </c>
+      <c r="F69" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>FREGADEROS DE COCINA</t>
+        </is>
+      </c>
+      <c r="C70" s="2" t="n">
+        <v>513.831046659336</v>
+      </c>
+      <c r="D70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2" t="n">
+        <v>513.831046659336</v>
+      </c>
+      <c r="F70" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>GRANITO</t>
+        </is>
+      </c>
+      <c r="C71" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="D71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="F71" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>GRIFERIAS</t>
+        </is>
+      </c>
+      <c r="C72" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="D72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="F72" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>INODOROS</t>
+        </is>
+      </c>
+      <c r="C73" s="2" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" s="2" t="n">
+        <v>1800</v>
+      </c>
+      <c r="F73" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>LAVABOS</t>
+        </is>
+      </c>
+      <c r="C74" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="D74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="F74" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="C75" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F75" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>NO RESURTIBLES</t>
+        </is>
+      </c>
+      <c r="C76" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="D76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="F76" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>PANELES DECORATIVOS</t>
+        </is>
+      </c>
+      <c r="C78" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="D78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F78" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>PANELES PU</t>
+        </is>
+      </c>
+      <c r="C79" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="D79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="F79" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>PANELES PVC</t>
+        </is>
+      </c>
+      <c r="C80" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="D80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E80" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="F80" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>PIEDRA SINTERIZADA</t>
+        </is>
+      </c>
+      <c r="C81" s="2" t="n">
+        <v>7465</v>
+      </c>
+      <c r="D81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E81" s="2" t="n">
+        <v>7465</v>
+      </c>
+      <c r="F81" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C82" s="2" t="n">
+        <v>29532.44</v>
+      </c>
+      <c r="D82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E82" s="2" t="n">
+        <v>29532.44</v>
+      </c>
+      <c r="F82" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>PUERTAS DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="C83" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="D83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E83" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="F83" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>SAL SOLUBLE</t>
+        </is>
+      </c>
+      <c r="C84" s="2" t="n">
+        <v>2800</v>
+      </c>
+      <c r="D84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E84" s="2" t="n">
+        <v>2800</v>
+      </c>
+      <c r="F84" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>240X120 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C85" s="2" t="n">
+        <v>672.340305337043</v>
+      </c>
+      <c r="D85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E85" s="2" t="n">
+        <v>672.340305337043</v>
+      </c>
+      <c r="F85" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>240X80 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C86" s="2" t="n">
+        <v>4992.1832</v>
+      </c>
+      <c r="D86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" s="2" t="n">
+        <v>4992.1832</v>
+      </c>
+      <c r="F86" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>FREGADEROS DE COCINA</t>
+        </is>
+      </c>
+      <c r="C87" s="2" t="n">
+        <v>142.502095025027</v>
+      </c>
+      <c r="D87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E87" s="2" t="n">
+        <v>142.502095025027</v>
+      </c>
+      <c r="F87" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>GRANITO</t>
+        </is>
+      </c>
+      <c r="C88" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="D88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E88" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="F88" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>GRIFERIAS</t>
+        </is>
+      </c>
+      <c r="C89" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="D89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E89" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="F89" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>INODOROS</t>
+        </is>
+      </c>
+      <c r="C90" s="2" t="n">
+        <v>2100</v>
+      </c>
+      <c r="D90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E90" s="2" t="n">
+        <v>2100</v>
+      </c>
+      <c r="F90" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>LAVABOS</t>
+        </is>
+      </c>
+      <c r="C91" s="2" t="n">
+        <v>750</v>
+      </c>
+      <c r="D91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E91" s="2" t="n">
+        <v>750</v>
+      </c>
+      <c r="F91" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="C92" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E92" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F92" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>NO RESURTIBLES</t>
+        </is>
+      </c>
+      <c r="C93" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="D93" s="2" t="n">
+        <v>9.58</v>
+      </c>
+      <c r="E93" s="2" t="n">
+        <v>640.67</v>
+      </c>
+      <c r="F93" s="5" t="n">
+        <v>0.01473279507881584</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F94" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>PANELES DECORATIVOS</t>
+        </is>
+      </c>
+      <c r="C95" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="D95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E95" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F95" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>PANELES PU</t>
+        </is>
+      </c>
+      <c r="C96" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="D96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E96" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="F96" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>PANELES PVC</t>
+        </is>
+      </c>
+      <c r="C97" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="D97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E97" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="F97" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>PIEDRA SINTERIZADA</t>
+        </is>
+      </c>
+      <c r="C98" s="2" t="n">
+        <v>1505.12</v>
+      </c>
+      <c r="D98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E98" s="2" t="n">
+        <v>1505.12</v>
+      </c>
+      <c r="F98" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C99" s="2" t="n">
+        <v>38417.17</v>
+      </c>
+      <c r="D99" s="2" t="n">
+        <v>233.38</v>
+      </c>
+      <c r="E99" s="2" t="n">
+        <v>38183.79</v>
+      </c>
+      <c r="F99" s="5" t="n">
+        <v>0.006074887869148092</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>PUERTAS DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="C100" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="D100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E100" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="F100" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>LINDAO ZUÑIGA BRYAN JOSE</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>SAL SOLUBLE</t>
+        </is>
+      </c>
+      <c r="C101" s="2" t="n">
+        <v>4130</v>
+      </c>
+      <c r="D101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E101" s="2" t="n">
+        <v>4130</v>
+      </c>
+      <c r="F101" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>240X120 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C102" s="2" t="n">
+        <v>344.284604629486</v>
+      </c>
+      <c r="D102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E102" s="2" t="n">
+        <v>344.284604629486</v>
+      </c>
+      <c r="F102" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>240X80 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C103" s="2" t="n">
+        <v>3120.1145</v>
+      </c>
+      <c r="D103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E103" s="2" t="n">
+        <v>3120.1145</v>
+      </c>
+      <c r="F103" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>FREGADEROS DE COCINA</t>
+        </is>
+      </c>
+      <c r="C104" s="2" t="n">
+        <v>250.631825420901</v>
+      </c>
+      <c r="D104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E104" s="2" t="n">
+        <v>250.631825420901</v>
+      </c>
+      <c r="F104" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>GRANITO</t>
+        </is>
+      </c>
+      <c r="C105" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="D105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E105" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="F105" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>GRIFERIAS</t>
+        </is>
+      </c>
+      <c r="C106" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="D106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E106" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="F106" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>INODOROS</t>
+        </is>
+      </c>
+      <c r="C107" s="2" t="n">
+        <v>560</v>
+      </c>
+      <c r="D107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E107" s="2" t="n">
+        <v>560</v>
+      </c>
+      <c r="F107" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>LAVABOS</t>
+        </is>
+      </c>
+      <c r="C108" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="D108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E108" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="F108" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="C109" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E109" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F109" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>NO RESURTIBLES</t>
+        </is>
+      </c>
+      <c r="C110" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="D110" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E110" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="F110" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F111" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>PANELES DECORATIVOS</t>
+        </is>
+      </c>
+      <c r="C112" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="D112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E112" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F112" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>PANELES PU</t>
+        </is>
+      </c>
+      <c r="C113" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="D113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E113" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="F113" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>PANELES PVC</t>
+        </is>
+      </c>
+      <c r="C114" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="D114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E114" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="F114" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>PIEDRA SINTERIZADA</t>
+        </is>
+      </c>
+      <c r="C115" s="2" t="n">
+        <v>1638</v>
+      </c>
+      <c r="D115" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E115" s="2" t="n">
+        <v>1638</v>
+      </c>
+      <c r="F115" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C116" s="2" t="n">
+        <v>13061.58</v>
+      </c>
+      <c r="D116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E116" s="2" t="n">
+        <v>13061.58</v>
+      </c>
+      <c r="F116" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>PUERTAS DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="C117" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="D117" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E117" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="F117" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>LOZANO MOLINA TITO</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>SAL SOLUBLE</t>
+        </is>
+      </c>
+      <c r="C118" s="2" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E118" s="2" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F118" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D119" s="2" t="n">
+        <v>605.48</v>
+      </c>
+      <c r="E119" s="2" t="n">
+        <v>-605.48</v>
+      </c>
+      <c r="F119" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>OFICINA-CATAECSA</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C120" s="2" t="n">
+        <v>17500</v>
+      </c>
+      <c r="D120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E120" s="2" t="n">
+        <v>17500</v>
+      </c>
+      <c r="F120" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>240X120 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C121" s="2" t="n">
+        <v>1041.16</v>
+      </c>
+      <c r="D121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E121" s="2" t="n">
+        <v>1041.16</v>
+      </c>
+      <c r="F121" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>240X80 PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C122" s="2" t="n">
+        <v>8668.91</v>
+      </c>
+      <c r="D122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E122" s="2" t="n">
+        <v>8668.91</v>
+      </c>
+      <c r="F122" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>FREGADEROS DE COCINA</t>
+        </is>
+      </c>
+      <c r="C123" s="2" t="n">
+        <v>372.993863046034</v>
+      </c>
+      <c r="D123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E123" s="2" t="n">
+        <v>372.993863046034</v>
+      </c>
+      <c r="F123" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>GRANITO</t>
+        </is>
+      </c>
+      <c r="C124" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="D124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E124" s="2" t="n">
+        <v>238.32</v>
+      </c>
+      <c r="F124" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>GRIFERIAS</t>
+        </is>
+      </c>
+      <c r="C125" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="D125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E125" s="2" t="n">
+        <v>106.82</v>
+      </c>
+      <c r="F125" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>INODOROS</t>
+        </is>
+      </c>
+      <c r="C126" s="2" t="n">
+        <v>800</v>
+      </c>
+      <c r="D126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E126" s="2" t="n">
+        <v>800</v>
+      </c>
+      <c r="F126" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>LAVABOS</t>
+        </is>
+      </c>
+      <c r="C127" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="D127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E127" s="2" t="n">
+        <v>625</v>
+      </c>
+      <c r="F127" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>LED</t>
+        </is>
+      </c>
+      <c r="C128" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="D128" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E128" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F128" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>NO RESURTIBLES</t>
+        </is>
+      </c>
+      <c r="C129" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="D129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E129" s="2" t="n">
+        <v>650.25</v>
+      </c>
+      <c r="F129" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>OTROS</t>
+        </is>
+      </c>
+      <c r="C130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F130" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>PANELES DECORATIVOS</t>
+        </is>
+      </c>
+      <c r="C131" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="D131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E131" s="2" t="n">
+        <v>350</v>
+      </c>
+      <c r="F131" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>PANELES PU</t>
+        </is>
+      </c>
+      <c r="C132" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="D132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E132" s="2" t="n">
+        <v>230</v>
+      </c>
+      <c r="F132" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>PANELES PVC</t>
+        </is>
+      </c>
+      <c r="C133" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="D133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E133" s="2" t="n">
+        <v>483</v>
+      </c>
+      <c r="F133" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>PIEDRA SINTERIZADA</t>
+        </is>
+      </c>
+      <c r="C134" s="2" t="n">
+        <v>2501.01</v>
+      </c>
+      <c r="D134" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E134" s="2" t="n">
+        <v>2501.01</v>
+      </c>
+      <c r="F134" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>PORCELANATO</t>
+        </is>
+      </c>
+      <c r="C135" s="2" t="n">
+        <v>28209.84</v>
+      </c>
+      <c r="D135" s="2" t="n">
+        <v>-22.68</v>
+      </c>
+      <c r="E135" s="2" t="n">
+        <v>28232.52</v>
+      </c>
+      <c r="F135" s="5" t="n">
+        <v>-0.0008039747832671153</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>PUERTAS DE SEGURIDAD</t>
+        </is>
+      </c>
+      <c r="C136" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="D136" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E136" s="2" t="n">
+        <v>342</v>
+      </c>
+      <c r="F136" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>RIOS CARRION ANGEL BENIGNO</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>SAL SOLUBLE</t>
+        </is>
+      </c>
+      <c r="C137" s="2" t="n">
+        <v>2300</v>
+      </c>
+      <c r="D137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E137" s="2" t="n">
+        <v>2300</v>
+      </c>
+      <c r="F137" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="B138" s="6" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="C138" s="2" t="n">
+        <v>422464.7705625342</v>
+      </c>
+      <c r="D138" s="2" t="n">
+        <v>8919.789999999999</v>
+      </c>
+      <c r="E138" s="2" t="n">
+        <v>413544.9805625342</v>
+      </c>
+      <c r="F138" s="5" t="n">
+        <v>0.0211136895228514</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización automática 2025-06-24 11:40:08
</commit_message>
<xml_diff>
--- a/data/STROBEL CORDERO MARIA ELISABETH.xlsx
+++ b/data/STROBEL CORDERO MARIA ELISABETH.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R270"/>
+  <dimension ref="A1:R271"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16588,137 +16588,197 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
+        </is>
+      </c>
+      <c r="C269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R269" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>VACA PANCHI CAROLINA</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
           <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
-      <c r="C269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R269" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="270">
-      <c r="C270" s="3" t="inlineStr">
-        <is>
-          <t>11 de 268</t>
-        </is>
-      </c>
-      <c r="D270" s="3" t="inlineStr">
-        <is>
-          <t>29 de 268</t>
-        </is>
-      </c>
-      <c r="E270" s="3" t="inlineStr">
-        <is>
-          <t>8 de 268</t>
-        </is>
-      </c>
-      <c r="F270" s="3" t="inlineStr">
-        <is>
-          <t>0 de 268</t>
-        </is>
-      </c>
-      <c r="G270" s="3" t="inlineStr">
-        <is>
-          <t>4 de 268</t>
-        </is>
-      </c>
-      <c r="H270" s="3" t="inlineStr">
-        <is>
-          <t>2 de 268</t>
-        </is>
-      </c>
-      <c r="I270" s="3" t="inlineStr">
-        <is>
-          <t>3 de 268</t>
-        </is>
-      </c>
-      <c r="J270" s="3" t="inlineStr">
-        <is>
-          <t>1 de 268</t>
-        </is>
-      </c>
-      <c r="K270" s="3" t="inlineStr">
-        <is>
-          <t>3 de 268</t>
-        </is>
-      </c>
-      <c r="L270" s="3" t="inlineStr">
-        <is>
-          <t>16 de 268</t>
-        </is>
-      </c>
-      <c r="M270" s="3" t="inlineStr">
-        <is>
-          <t>33 de 268</t>
-        </is>
-      </c>
-      <c r="N270" s="3" t="inlineStr">
-        <is>
-          <t>2 de 268</t>
-        </is>
-      </c>
-      <c r="O270" s="3" t="inlineStr">
-        <is>
-          <t>6 de 268</t>
-        </is>
-      </c>
-      <c r="P270" s="3" t="inlineStr">
-        <is>
-          <t>8 de 268</t>
-        </is>
-      </c>
-      <c r="Q270" s="3" t="inlineStr">
-        <is>
-          <t>7 de 268</t>
-        </is>
-      </c>
-      <c r="R270" s="3" t="inlineStr">
-        <is>
-          <t>2 de 268</t>
+      <c r="C270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R270" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="C271" s="3" t="inlineStr">
+        <is>
+          <t>11 de 269</t>
+        </is>
+      </c>
+      <c r="D271" s="3" t="inlineStr">
+        <is>
+          <t>29 de 269</t>
+        </is>
+      </c>
+      <c r="E271" s="3" t="inlineStr">
+        <is>
+          <t>8 de 269</t>
+        </is>
+      </c>
+      <c r="F271" s="3" t="inlineStr">
+        <is>
+          <t>0 de 269</t>
+        </is>
+      </c>
+      <c r="G271" s="3" t="inlineStr">
+        <is>
+          <t>4 de 269</t>
+        </is>
+      </c>
+      <c r="H271" s="3" t="inlineStr">
+        <is>
+          <t>2 de 269</t>
+        </is>
+      </c>
+      <c r="I271" s="3" t="inlineStr">
+        <is>
+          <t>3 de 269</t>
+        </is>
+      </c>
+      <c r="J271" s="3" t="inlineStr">
+        <is>
+          <t>1 de 269</t>
+        </is>
+      </c>
+      <c r="K271" s="3" t="inlineStr">
+        <is>
+          <t>3 de 269</t>
+        </is>
+      </c>
+      <c r="L271" s="3" t="inlineStr">
+        <is>
+          <t>16 de 269</t>
+        </is>
+      </c>
+      <c r="M271" s="3" t="inlineStr">
+        <is>
+          <t>33 de 269</t>
+        </is>
+      </c>
+      <c r="N271" s="3" t="inlineStr">
+        <is>
+          <t>2 de 269</t>
+        </is>
+      </c>
+      <c r="O271" s="3" t="inlineStr">
+        <is>
+          <t>6 de 269</t>
+        </is>
+      </c>
+      <c r="P271" s="3" t="inlineStr">
+        <is>
+          <t>8 de 269</t>
+        </is>
+      </c>
+      <c r="Q271" s="3" t="inlineStr">
+        <is>
+          <t>7 de 269</t>
+        </is>
+      </c>
+      <c r="R271" s="3" t="inlineStr">
+        <is>
+          <t>2 de 269</t>
         </is>
       </c>
     </row>
@@ -16733,7 +16793,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G270"/>
+  <dimension ref="A1:G272"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23977,7 +24037,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+          <t>KITCHENSCO S.A.</t>
         </is>
       </c>
       <c r="C268" s="2" t="n">
@@ -24004,39 +24064,93 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+        </is>
+      </c>
+      <c r="C269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F269" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G269" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>VACA PANCHI CAROLINA</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
+        </is>
+      </c>
+      <c r="C270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G270" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>VACA PANCHI CAROLINA</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
           <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
-      <c r="C269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D269" s="2" t="n">
+      <c r="C271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D271" s="2" t="n">
         <v>3.47</v>
       </c>
-      <c r="E269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F269" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G269" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="270">
-      <c r="C270" s="4" t="n">
+      <c r="E271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G271" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="C272" s="4" t="n">
         <v>348971.25</v>
       </c>
-      <c r="D270" s="4" t="n">
+      <c r="D272" s="4" t="n">
         <v>250720.98</v>
       </c>
-      <c r="E270" s="4" t="n">
+      <c r="E272" s="4" t="n">
         <v>328974.99</v>
       </c>
-      <c r="F270" s="4" t="n">
+      <c r="F272" s="4" t="n">
         <v>176647.41</v>
       </c>
-      <c r="G270" s="4" t="n">
+      <c r="G272" s="4" t="n">
         <v>300500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-06-24 11:45:08
</commit_message>
<xml_diff>
--- a/data/STROBEL CORDERO MARIA ELISABETH.xlsx
+++ b/data/STROBEL CORDERO MARIA ELISABETH.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R271"/>
+  <dimension ref="A1:R273"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16528,7 +16528,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+          <t>KITCHENSCO S.A.</t>
         </is>
       </c>
       <c r="C268" s="2" t="n">
@@ -16588,7 +16588,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>PAREDES POVEDA TATIANA VERONICA</t>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
         </is>
       </c>
       <c r="C269" s="2" t="n">
@@ -16648,137 +16648,257 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
+        </is>
+      </c>
+      <c r="C270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q270" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R270" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>VACA PANCHI CAROLINA</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
           <t>VACA PANCHI DORYS CAROLINA</t>
         </is>
       </c>
-      <c r="C270" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D270" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E270" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F270" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G270" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H270" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I270" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J270" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K270" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L270" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M270" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N270" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O270" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P270" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q270" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R270" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="271">
-      <c r="C271" s="3" t="inlineStr">
-        <is>
-          <t>11 de 269</t>
-        </is>
-      </c>
-      <c r="D271" s="3" t="inlineStr">
-        <is>
-          <t>29 de 269</t>
-        </is>
-      </c>
-      <c r="E271" s="3" t="inlineStr">
-        <is>
-          <t>8 de 269</t>
-        </is>
-      </c>
-      <c r="F271" s="3" t="inlineStr">
-        <is>
-          <t>0 de 269</t>
-        </is>
-      </c>
-      <c r="G271" s="3" t="inlineStr">
-        <is>
-          <t>4 de 269</t>
-        </is>
-      </c>
-      <c r="H271" s="3" t="inlineStr">
-        <is>
-          <t>2 de 269</t>
-        </is>
-      </c>
-      <c r="I271" s="3" t="inlineStr">
-        <is>
-          <t>3 de 269</t>
-        </is>
-      </c>
-      <c r="J271" s="3" t="inlineStr">
-        <is>
-          <t>1 de 269</t>
-        </is>
-      </c>
-      <c r="K271" s="3" t="inlineStr">
-        <is>
-          <t>3 de 269</t>
-        </is>
-      </c>
-      <c r="L271" s="3" t="inlineStr">
-        <is>
-          <t>16 de 269</t>
-        </is>
-      </c>
-      <c r="M271" s="3" t="inlineStr">
-        <is>
-          <t>33 de 269</t>
-        </is>
-      </c>
-      <c r="N271" s="3" t="inlineStr">
-        <is>
-          <t>2 de 269</t>
-        </is>
-      </c>
-      <c r="O271" s="3" t="inlineStr">
-        <is>
-          <t>6 de 269</t>
-        </is>
-      </c>
-      <c r="P271" s="3" t="inlineStr">
-        <is>
-          <t>8 de 269</t>
-        </is>
-      </c>
-      <c r="Q271" s="3" t="inlineStr">
-        <is>
-          <t>7 de 269</t>
-        </is>
-      </c>
-      <c r="R271" s="3" t="inlineStr">
-        <is>
-          <t>2 de 269</t>
+      <c r="C271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q271" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R271" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>VACA PANCHI CAROLINA</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R272" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="C273" s="3" t="inlineStr">
+        <is>
+          <t>11 de 271</t>
+        </is>
+      </c>
+      <c r="D273" s="3" t="inlineStr">
+        <is>
+          <t>29 de 271</t>
+        </is>
+      </c>
+      <c r="E273" s="3" t="inlineStr">
+        <is>
+          <t>8 de 271</t>
+        </is>
+      </c>
+      <c r="F273" s="3" t="inlineStr">
+        <is>
+          <t>0 de 271</t>
+        </is>
+      </c>
+      <c r="G273" s="3" t="inlineStr">
+        <is>
+          <t>4 de 271</t>
+        </is>
+      </c>
+      <c r="H273" s="3" t="inlineStr">
+        <is>
+          <t>2 de 271</t>
+        </is>
+      </c>
+      <c r="I273" s="3" t="inlineStr">
+        <is>
+          <t>3 de 271</t>
+        </is>
+      </c>
+      <c r="J273" s="3" t="inlineStr">
+        <is>
+          <t>1 de 271</t>
+        </is>
+      </c>
+      <c r="K273" s="3" t="inlineStr">
+        <is>
+          <t>3 de 271</t>
+        </is>
+      </c>
+      <c r="L273" s="3" t="inlineStr">
+        <is>
+          <t>16 de 271</t>
+        </is>
+      </c>
+      <c r="M273" s="3" t="inlineStr">
+        <is>
+          <t>33 de 271</t>
+        </is>
+      </c>
+      <c r="N273" s="3" t="inlineStr">
+        <is>
+          <t>2 de 271</t>
+        </is>
+      </c>
+      <c r="O273" s="3" t="inlineStr">
+        <is>
+          <t>6 de 271</t>
+        </is>
+      </c>
+      <c r="P273" s="3" t="inlineStr">
+        <is>
+          <t>8 de 271</t>
+        </is>
+      </c>
+      <c r="Q273" s="3" t="inlineStr">
+        <is>
+          <t>7 de 271</t>
+        </is>
+      </c>
+      <c r="R273" s="3" t="inlineStr">
+        <is>
+          <t>2 de 271</t>
         </is>
       </c>
     </row>
@@ -16793,7 +16913,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G272"/>
+  <dimension ref="A1:G273"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24138,19 +24258,46 @@
       </c>
     </row>
     <row r="272">
-      <c r="C272" s="4" t="n">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>VACA PANCHI CAROLINA</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>VIZUETE GALARZA EDWIN RODRIGO</t>
+        </is>
+      </c>
+      <c r="C272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F272" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G272" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="C273" s="4" t="n">
         <v>348971.25</v>
       </c>
-      <c r="D272" s="4" t="n">
+      <c r="D273" s="4" t="n">
         <v>250720.98</v>
       </c>
-      <c r="E272" s="4" t="n">
+      <c r="E273" s="4" t="n">
         <v>328974.99</v>
       </c>
-      <c r="F272" s="4" t="n">
+      <c r="F273" s="4" t="n">
         <v>176647.41</v>
       </c>
-      <c r="G272" s="4" t="n">
+      <c r="G273" s="4" t="n">
         <v>300500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-07-18 16:55:09
</commit_message>
<xml_diff>
--- a/data/STROBEL CORDERO MARIA ELISABETH.xlsx
+++ b/data/STROBEL CORDERO MARIA ELISABETH.xlsx
@@ -440,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R284"/>
+  <dimension ref="A1:R285"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17188,7 +17188,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>KITCHENSCO S.A.</t>
+          <t>GRANJA VANEGAS MARCELA</t>
         </is>
       </c>
       <c r="C279" s="2" t="n">
@@ -17248,7 +17248,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+          <t>KITCHENSCO S.A.</t>
         </is>
       </c>
       <c r="C280" s="2" t="n">
@@ -17308,7 +17308,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>PAREDES POVEDA TATIANA VERONICA</t>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
         </is>
       </c>
       <c r="C281" s="2" t="n">
@@ -17368,7 +17368,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
         </is>
       </c>
       <c r="C282" s="2" t="n">
@@ -17428,137 +17428,197 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
+          <t>VACA PANCHI DORYS CAROLINA</t>
+        </is>
+      </c>
+      <c r="C283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R283" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>VACA PANCHI CAROLINA</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
           <t>VIZUETE GALARZA EDWIN RODRIGO</t>
         </is>
       </c>
-      <c r="C283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R283" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="284">
-      <c r="C284" s="3" t="inlineStr">
-        <is>
-          <t>4 de 282</t>
-        </is>
-      </c>
-      <c r="D284" s="3" t="inlineStr">
-        <is>
-          <t>10 de 282</t>
-        </is>
-      </c>
-      <c r="E284" s="3" t="inlineStr">
-        <is>
-          <t>10 de 282</t>
-        </is>
-      </c>
-      <c r="F284" s="3" t="inlineStr">
-        <is>
-          <t>1 de 282</t>
-        </is>
-      </c>
-      <c r="G284" s="3" t="inlineStr">
-        <is>
-          <t>0 de 282</t>
-        </is>
-      </c>
-      <c r="H284" s="3" t="inlineStr">
-        <is>
-          <t>9 de 282</t>
-        </is>
-      </c>
-      <c r="I284" s="3" t="inlineStr">
-        <is>
-          <t>13 de 282</t>
-        </is>
-      </c>
-      <c r="J284" s="3" t="inlineStr">
-        <is>
-          <t>0 de 282</t>
-        </is>
-      </c>
-      <c r="K284" s="3" t="inlineStr">
-        <is>
-          <t>1 de 282</t>
-        </is>
-      </c>
-      <c r="L284" s="3" t="inlineStr">
-        <is>
-          <t>11 de 282</t>
-        </is>
-      </c>
-      <c r="M284" s="3" t="inlineStr">
-        <is>
-          <t>50 de 282</t>
-        </is>
-      </c>
-      <c r="N284" s="3" t="inlineStr">
-        <is>
-          <t>2 de 282</t>
-        </is>
-      </c>
-      <c r="O284" s="3" t="inlineStr">
-        <is>
-          <t>3 de 282</t>
-        </is>
-      </c>
-      <c r="P284" s="3" t="inlineStr">
-        <is>
-          <t>3 de 282</t>
-        </is>
-      </c>
-      <c r="Q284" s="3" t="inlineStr">
-        <is>
-          <t>5 de 282</t>
-        </is>
-      </c>
-      <c r="R284" s="3" t="inlineStr">
-        <is>
-          <t>0 de 282</t>
+      <c r="C284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R284" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="C285" s="3" t="inlineStr">
+        <is>
+          <t>4 de 283</t>
+        </is>
+      </c>
+      <c r="D285" s="3" t="inlineStr">
+        <is>
+          <t>10 de 283</t>
+        </is>
+      </c>
+      <c r="E285" s="3" t="inlineStr">
+        <is>
+          <t>10 de 283</t>
+        </is>
+      </c>
+      <c r="F285" s="3" t="inlineStr">
+        <is>
+          <t>1 de 283</t>
+        </is>
+      </c>
+      <c r="G285" s="3" t="inlineStr">
+        <is>
+          <t>0 de 283</t>
+        </is>
+      </c>
+      <c r="H285" s="3" t="inlineStr">
+        <is>
+          <t>9 de 283</t>
+        </is>
+      </c>
+      <c r="I285" s="3" t="inlineStr">
+        <is>
+          <t>13 de 283</t>
+        </is>
+      </c>
+      <c r="J285" s="3" t="inlineStr">
+        <is>
+          <t>0 de 283</t>
+        </is>
+      </c>
+      <c r="K285" s="3" t="inlineStr">
+        <is>
+          <t>1 de 283</t>
+        </is>
+      </c>
+      <c r="L285" s="3" t="inlineStr">
+        <is>
+          <t>11 de 283</t>
+        </is>
+      </c>
+      <c r="M285" s="3" t="inlineStr">
+        <is>
+          <t>50 de 283</t>
+        </is>
+      </c>
+      <c r="N285" s="3" t="inlineStr">
+        <is>
+          <t>2 de 283</t>
+        </is>
+      </c>
+      <c r="O285" s="3" t="inlineStr">
+        <is>
+          <t>3 de 283</t>
+        </is>
+      </c>
+      <c r="P285" s="3" t="inlineStr">
+        <is>
+          <t>3 de 283</t>
+        </is>
+      </c>
+      <c r="Q285" s="3" t="inlineStr">
+        <is>
+          <t>5 de 283</t>
+        </is>
+      </c>
+      <c r="R285" s="3" t="inlineStr">
+        <is>
+          <t>0 de 283</t>
         </is>
       </c>
     </row>
@@ -17573,7 +17633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G284"/>
+  <dimension ref="A1:G285"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25114,7 +25174,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>KITCHENSCO S.A.</t>
+          <t>GRANJA VANEGAS MARCELA</t>
         </is>
       </c>
       <c r="C279" s="2" t="n">
@@ -25141,7 +25201,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
+          <t>KITCHENSCO S.A.</t>
         </is>
       </c>
       <c r="C280" s="2" t="n">
@@ -25168,7 +25228,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>PAREDES POVEDA TATIANA VERONICA</t>
+          <t>LINCANGO LUGMANIA SANDY LIZETH</t>
         </is>
       </c>
       <c r="C281" s="2" t="n">
@@ -25195,17 +25255,17 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>VACA PANCHI DORYS CAROLINA</t>
+          <t>PAREDES POVEDA TATIANA VERONICA</t>
         </is>
       </c>
       <c r="C282" s="2" t="n">
-        <v>3.47</v>
+        <v>0</v>
       </c>
       <c r="D282" s="2" t="n">
         <v>0</v>
       </c>
       <c r="E282" s="2" t="n">
-        <v>10.44</v>
+        <v>0</v>
       </c>
       <c r="F282" s="2" t="n">
         <v>0</v>
@@ -25222,39 +25282,66 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
+          <t>VACA PANCHI DORYS CAROLINA</t>
+        </is>
+      </c>
+      <c r="C283" s="2" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="D283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E283" s="2" t="n">
+        <v>10.44</v>
+      </c>
+      <c r="F283" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G283" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>VACA PANCHI CAROLINA</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
           <t>VIZUETE GALARZA EDWIN RODRIGO</t>
         </is>
       </c>
-      <c r="C283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F283" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G283" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="284">
-      <c r="C284" s="4" t="n">
+      <c r="C284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F284" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G284" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="C285" s="4" t="n">
         <v>250720.98</v>
       </c>
-      <c r="D284" s="4" t="n">
+      <c r="D285" s="4" t="n">
         <v>328974.99</v>
       </c>
-      <c r="E284" s="4" t="n">
+      <c r="E285" s="4" t="n">
         <v>325882.43</v>
       </c>
-      <c r="F284" s="4" t="n">
+      <c r="F285" s="4" t="n">
         <v>165192.09</v>
       </c>
-      <c r="G284" s="4" t="n">
+      <c r="G285" s="4" t="n">
         <v>440476</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-12-03 15:30:07
</commit_message>
<xml_diff>
--- a/data/STROBEL CORDERO MARIA ELISABETH.xlsx
+++ b/data/STROBEL CORDERO MARIA ELISABETH.xlsx
@@ -5879,7 +5879,7 @@
         <v>0</v>
       </c>
       <c r="L90" s="2" t="n">
-        <v>0</v>
+        <v>447.78</v>
       </c>
       <c r="M90" s="2" t="n">
         <v>0</v>
@@ -22028,7 +22028,7 @@
       </c>
       <c r="L359" s="3" t="inlineStr">
         <is>
-          <t>7 de 357</t>
+          <t>8 de 357</t>
         </is>
       </c>
       <c r="M359" s="3" t="inlineStr">
@@ -24524,7 +24524,7 @@
         <v>0</v>
       </c>
       <c r="F90" s="2" t="n">
-        <v>0</v>
+        <v>447.78</v>
       </c>
       <c r="G90" s="2" t="n">
         <v>2000</v>
@@ -31885,7 +31885,7 @@
         <v>412473.7</v>
       </c>
       <c r="F363" s="4" t="n">
-        <v>29418.85</v>
+        <v>29866.63</v>
       </c>
       <c r="G363" s="4" t="n">
         <v>391124.88</v>

</xml_diff>